<commit_message>
fixed "0" event scores. Attempted to fix issue with github action
</commit_message>
<xml_diff>
--- a/input/scores.xlsx
+++ b/input/scores.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G96"/>
+  <dimension ref="A1:G164"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -474,24 +474,24 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>95</v>
+        <v>163</v>
       </c>
       <c r="C2" s="2" t="n">
-        <v>45877</v>
+        <v>46038</v>
       </c>
       <c r="D2" t="n">
-        <v>-4</v>
+        <v>-15</v>
       </c>
       <c r="E2" t="n">
-        <v>-94</v>
+        <v>-340</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>https://washingtoncitypaper.com/article/769029/the-needle-feds-patrolling-d-c-streets-pirro-calls-on-d-c-council-to-repeal-restorative-justice-laws-and-trans-air-force-members-lose-retirement-benefits/</t>
+          <t>https://washingtoncitypaper.com/article/777681/needle-ice-vetting-training-white-supremacist-prosecutor-texas-trump-nobel-prize/</t>
         </is>
       </c>
       <c r="G2" t="n">
-        <v>-90</v>
+        <v>-325</v>
       </c>
     </row>
     <row r="3">
@@ -499,24 +499,24 @@
         <v>0</v>
       </c>
       <c r="B3" t="n">
-        <v>94</v>
+        <v>162</v>
       </c>
       <c r="C3" s="2" t="n">
-        <v>45876</v>
+        <v>46037</v>
       </c>
       <c r="D3" t="n">
-        <v>-2</v>
+        <v>-30</v>
       </c>
       <c r="E3" t="n">
-        <v>-90</v>
+        <v>-325</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>https://washingtoncitypaper.com/article/768905/trumps-remaking-the-criminal-justice-system-and-14-states-plus-d-c-sue-for-gender-affirming-care/</t>
+          <t>https://washingtoncitypaper.com/article/777630/the-needle-another-ice-shooting-in-minnesota-more-nazi-imagery-from-the-trump-admin-and-bezos-remains-silent-on-fbi-raid/</t>
         </is>
       </c>
       <c r="G3" t="n">
-        <v>-88</v>
+        <v>-320</v>
       </c>
     </row>
     <row r="4">
@@ -524,24 +524,24 @@
         <v>0</v>
       </c>
       <c r="B4" t="n">
-        <v>93</v>
+        <v>161</v>
       </c>
       <c r="C4" s="2" t="n">
-        <v>45875</v>
+        <v>46035</v>
       </c>
       <c r="D4" t="n">
-        <v>-6</v>
+        <v>-7</v>
       </c>
       <c r="E4" t="n">
-        <v>-88</v>
+        <v>-320</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>https://washingtoncitypaper.com/article/768849/needle-big-balls-assault-federal-takeover-family-separations/</t>
+          <t>https://washingtoncitypaper.com/article/777472/needle-pentagon-disguised-aircraft-doj-refuses-investigate-shooting-minneapolis/</t>
         </is>
       </c>
       <c r="G4" t="n">
-        <v>-76</v>
+        <v>-313</v>
       </c>
     </row>
     <row r="5">
@@ -549,24 +549,24 @@
         <v>0</v>
       </c>
       <c r="B5" t="n">
-        <v>92</v>
+        <v>160</v>
       </c>
       <c r="C5" s="2" t="n">
-        <v>45869</v>
+        <v>46034</v>
       </c>
       <c r="D5" t="n">
-        <v>-2</v>
+        <v>-15</v>
       </c>
       <c r="E5" t="n">
-        <v>-76</v>
+        <v>-313</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>https://washingtoncitypaper.com/article/768593/needle-social-security-epstein-layoffs-buyout-ice/</t>
+          <t>https://washingtoncitypaper.com/article/777373/needle-trump-investigating-fed-chair-portrait-gallery-removed-trumps-impeachments/</t>
         </is>
       </c>
       <c r="G5" t="n">
-        <v>-65</v>
+        <v>-298</v>
       </c>
     </row>
     <row r="6">
@@ -574,24 +574,24 @@
         <v>0</v>
       </c>
       <c r="B6" t="n">
-        <v>91</v>
+        <v>159</v>
       </c>
       <c r="C6" s="2" t="n">
-        <v>45866</v>
+        <v>46031</v>
       </c>
       <c r="D6" t="n">
-        <v>-3</v>
+        <v>-8</v>
       </c>
       <c r="E6" t="n">
-        <v>-65</v>
+        <v>-298</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>https://washingtoncitypaper.com/article/768370/needle-scotland-troll-trump-qatar-jet-darren-beattie/</t>
+          <t>https://washingtoncitypaper.com/article/777237/needle-mpd-ice-bowser-portland-border-patrol-shooting/</t>
         </is>
       </c>
       <c r="G6" t="n">
-        <v>-62</v>
+        <v>-290</v>
       </c>
     </row>
     <row r="7">
@@ -599,24 +599,24 @@
         <v>0</v>
       </c>
       <c r="B7" t="n">
-        <v>90</v>
+        <v>158</v>
       </c>
       <c r="C7" s="2" t="n">
-        <v>45863</v>
+        <v>46030</v>
       </c>
       <c r="D7" t="n">
-        <v>0</v>
+        <v>-18</v>
       </c>
       <c r="E7" t="n">
-        <v>-62</v>
+        <v>-290</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>https://washingtoncitypaper.com/article/768303/needle-trump-republicans-oil-and-gas-companies-immigration-lawsuit/</t>
+          <t>https://washingtoncitypaper.com/article/777181/needle-ice-agent-killed-woman-minneapolis-video-contradicts-trump/</t>
         </is>
       </c>
       <c r="G7" t="n">
-        <v>-62</v>
+        <v>-272</v>
       </c>
     </row>
     <row r="8">
@@ -624,24 +624,24 @@
         <v>0</v>
       </c>
       <c r="B8" t="n">
-        <v>89</v>
+        <v>157</v>
       </c>
       <c r="C8" s="2" t="n">
-        <v>45862</v>
+        <v>46029</v>
       </c>
       <c r="D8" t="n">
-        <v>-1</v>
+        <v>7</v>
       </c>
       <c r="E8" t="n">
-        <v>-62</v>
+        <v>-272</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>https://washingtoncitypaper.com/article/768246/needle-weed-park-police-arrests/</t>
+          <t>https://washingtoncitypaper.com/article/777114/needle-trump-jan-6-lies-impeached-if-republicans-lose-house/</t>
         </is>
       </c>
       <c r="G8" t="n">
-        <v>-61</v>
+        <v>-279</v>
       </c>
     </row>
     <row r="9">
@@ -649,24 +649,24 @@
         <v>0</v>
       </c>
       <c r="B9" t="n">
-        <v>88</v>
+        <v>156</v>
       </c>
       <c r="C9" s="2" t="n">
-        <v>45861</v>
+        <v>46028</v>
       </c>
       <c r="D9" t="n">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="E9" t="n">
-        <v>-61</v>
+        <v>-279</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>https://washingtoncitypaper.com/article/768177/needle-ice-kids-feds-capitol-hill/</t>
+          <t>https://washingtoncitypaper.com/article/777007/needle-rioters-return-cop-teaching-history-nps-finally-fix-fountains/</t>
         </is>
       </c>
       <c r="G9" t="n">
-        <v>-66</v>
+        <v>-293</v>
       </c>
     </row>
     <row r="10">
@@ -674,24 +674,24 @@
         <v>0</v>
       </c>
       <c r="B10" t="n">
-        <v>87</v>
+        <v>155</v>
       </c>
       <c r="C10" s="2" t="n">
-        <v>45860</v>
+        <v>46014</v>
       </c>
       <c r="D10" t="n">
-        <v>-3</v>
+        <v>8</v>
       </c>
       <c r="E10" t="n">
-        <v>-66</v>
+        <v>-293</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>https://washingtoncitypaper.com/article/768121/needle-trump-distract-epstein/</t>
+          <t>https://washingtoncitypaper.com/article/776489/needle-trump-name-kennedy-center-doj-d-c-police-ar-15/</t>
         </is>
       </c>
       <c r="G10" t="n">
-        <v>-63</v>
+        <v>-301</v>
       </c>
     </row>
     <row r="11">
@@ -699,24 +699,24 @@
         <v>0</v>
       </c>
       <c r="B11" t="n">
-        <v>86</v>
+        <v>154</v>
       </c>
       <c r="C11" s="2" t="n">
-        <v>45859</v>
+        <v>46013</v>
       </c>
       <c r="D11" t="n">
-        <v>-2</v>
+        <v>-9</v>
       </c>
       <c r="E11" t="n">
-        <v>-63</v>
+        <v>-301</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>https://washingtoncitypaper.com/article/768062/the-needle-trump-says-rename-the-commanders-or-else-and-the-presidents-history-of-doodling/</t>
+          <t>https://washingtoncitypaper.com/article/776294/needle-dems-report-mpd-crime-stats-60-minutes-prison-jd-vance-bigots-conservative/</t>
         </is>
       </c>
       <c r="G11" t="n">
-        <v>-61</v>
+        <v>-292</v>
       </c>
     </row>
     <row r="12">
@@ -724,24 +724,24 @@
         <v>0</v>
       </c>
       <c r="B12" t="n">
-        <v>85</v>
+        <v>153</v>
       </c>
       <c r="C12" s="2" t="n">
-        <v>45856</v>
+        <v>46010</v>
       </c>
       <c r="D12" t="n">
-        <v>-5</v>
+        <v>-3</v>
       </c>
       <c r="E12" t="n">
-        <v>-61</v>
+        <v>-292</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>https://washingtoncitypaper.com/article/768013/the-needle-lgbtqia-youth-hotline-is-disconnected-and-ice-gets-access-to-medicaid-records/</t>
+          <t>https://washingtoncitypaper.com/article/776138/the-needle-trump-adds-his-name-to-the-kennedy-center-erika-kirk-endorses-vance-for-2028-and-americas-250th-birthday-celebration-is-giving-hunger-games/</t>
         </is>
       </c>
       <c r="G12" t="n">
-        <v>-56</v>
+        <v>-282</v>
       </c>
     </row>
     <row r="13">
@@ -749,24 +749,24 @@
         <v>0</v>
       </c>
       <c r="B13" t="n">
-        <v>84</v>
+        <v>152</v>
       </c>
       <c r="C13" s="2" t="n">
-        <v>45855</v>
+        <v>46008</v>
       </c>
       <c r="D13" t="n">
         <v>-1</v>
       </c>
       <c r="E13" t="n">
-        <v>-56</v>
+        <v>-282</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>https://washingtoncitypaper.com/article/767964/the-needle-protest-civil-rights-rollback-convention-industry-hit/</t>
+          <t>https://washingtoncitypaper.com/article/776030/the-needle-susie-wiles-dishes-usaid-cuts-led-to-deaths-despite-marco-rubios-claims-otherwise-and-coast-guard-calls-swastikas-and-nooses-potentially-divisive/</t>
         </is>
       </c>
       <c r="G13" t="n">
-        <v>-55</v>
+        <v>-273</v>
       </c>
     </row>
     <row r="14">
@@ -774,24 +774,24 @@
         <v>0</v>
       </c>
       <c r="B14" t="n">
-        <v>83</v>
+        <v>151</v>
       </c>
       <c r="C14" s="2" t="n">
-        <v>45854</v>
+        <v>46006</v>
       </c>
       <c r="D14" t="n">
-        <v>1</v>
+        <v>-7</v>
       </c>
       <c r="E14" t="n">
-        <v>-55</v>
+        <v>-273</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>https://washingtoncitypaper.com/article/767861/needle-inflation-speaker-johnson-epstein-protest/</t>
+          <t>https://washingtoncitypaper.com/article/775809/needle-tsa-ice-names-trump-deadnaming-asst-secretary-for-health/</t>
         </is>
       </c>
       <c r="G14" t="n">
-        <v>-56</v>
+        <v>-277</v>
       </c>
     </row>
     <row r="15">
@@ -799,24 +799,24 @@
         <v>0</v>
       </c>
       <c r="B15" t="n">
-        <v>82</v>
+        <v>150</v>
       </c>
       <c r="C15" s="2" t="n">
-        <v>45853</v>
+        <v>46000</v>
       </c>
       <c r="D15" t="n">
-        <v>1</v>
+        <v>-8</v>
       </c>
       <c r="E15" t="n">
-        <v>-56</v>
+        <v>-277</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>https://washingtoncitypaper.com/article/767762/needle-detained-migrants-maga-epstein-education-department/</t>
+          <t>https://washingtoncitypaper.com/article/775495/the-needle-trumps-policies-harm-d-c-restaurants-despite-his-claims-12-billion-farmer-bailout-undermines-tariffs-and-congress-ramps-up-scrutiny-of-deadly-boat-strikes/</t>
         </is>
       </c>
       <c r="G15" t="n">
-        <v>-57</v>
+        <v>-269</v>
       </c>
     </row>
     <row r="16">
@@ -824,24 +824,24 @@
         <v>0</v>
       </c>
       <c r="B16" t="n">
-        <v>81</v>
+        <v>149</v>
       </c>
       <c r="C16" s="2" t="n">
-        <v>45852</v>
+        <v>45999</v>
       </c>
       <c r="D16" t="n">
-        <v>0</v>
+        <v>-9</v>
       </c>
       <c r="E16" t="n">
-        <v>-57</v>
+        <v>-269</v>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>https://washingtoncitypaper.com/article/767708/the-needle-usao-spokesperson-fired-trump-booed-in-jersey-and-rosie-odonnell-claps-back/</t>
+          <t>https://washingtoncitypaper.com/article/775450/the-needle-trump-pardons-bigtime-drug-traffickers-the-supreme-court-considers-if-he-can-fire-federal-officials-and-cost-of-health-insurance-rises/</t>
         </is>
       </c>
       <c r="G16" t="n">
-        <v>-63</v>
+        <v>-260</v>
       </c>
     </row>
     <row r="17">
@@ -849,24 +849,24 @@
         <v>0</v>
       </c>
       <c r="B17" t="n">
-        <v>80</v>
+        <v>148</v>
       </c>
       <c r="C17" s="2" t="n">
-        <v>45848</v>
+        <v>45996</v>
       </c>
       <c r="D17" t="n">
-        <v>0</v>
+        <v>-12</v>
       </c>
       <c r="E17" t="n">
-        <v>-63</v>
+        <v>-260</v>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>https://washingtoncitypaper.com/article/767546/needle-trump-english-liberia-research/</t>
+          <t>https://washingtoncitypaper.com/article/775374/the-needle-partisan-responses-to-horrifying-boat-killing-video-and-mlk-day-and-juneteenth-removed-as-free-national-park-days/</t>
         </is>
       </c>
       <c r="G17" t="n">
-        <v>-61</v>
+        <v>-248</v>
       </c>
     </row>
     <row r="18">
@@ -874,24 +874,24 @@
         <v>0</v>
       </c>
       <c r="B18" t="n">
-        <v>79</v>
+        <v>147</v>
       </c>
       <c r="C18" s="2" t="n">
-        <v>45845</v>
+        <v>45995</v>
       </c>
       <c r="D18" t="n">
         <v>-4</v>
       </c>
       <c r="E18" t="n">
-        <v>-61</v>
+        <v>-248</v>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>https://washingtoncitypaper.com/article/767316/the-needle-tens-of-thousands-in-d-c-will-lose-health-coverage-under-trumps-big-bill/</t>
+          <t>https://washingtoncitypaper.com/article/775302/the-needle-hegseth-endangered-troops-with-group-chat-leak-and-most-arrested-by-ice-in-d-c-had-no-criminal-record/</t>
         </is>
       </c>
       <c r="G18" t="n">
-        <v>-54</v>
+        <v>-244</v>
       </c>
     </row>
     <row r="19">
@@ -899,24 +899,24 @@
         <v>0</v>
       </c>
       <c r="B19" t="n">
-        <v>78</v>
+        <v>146</v>
       </c>
       <c r="C19" s="2" t="n">
-        <v>45840</v>
+        <v>45994</v>
       </c>
       <c r="D19" t="n">
-        <v>-3</v>
+        <v>-5</v>
       </c>
       <c r="E19" t="n">
-        <v>-54</v>
+        <v>-244</v>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>https://washingtoncitypaper.com/article/767067/needle-health-insurance-senate-anacostia-community-museum/</t>
+          <t>https://washingtoncitypaper.com/article/775189/needle-trump-racist-hegseth-fog-of-war-judge-stop-warrantless-arrests/</t>
         </is>
       </c>
       <c r="G19" t="n">
-        <v>-51</v>
+        <v>-239</v>
       </c>
     </row>
     <row r="20">
@@ -924,24 +924,24 @@
         <v>0</v>
       </c>
       <c r="B20" t="n">
-        <v>77</v>
+        <v>145</v>
       </c>
       <c r="C20" s="2" t="n">
-        <v>45839</v>
+        <v>45993</v>
       </c>
       <c r="D20" t="n">
-        <v>-2</v>
+        <v>1</v>
       </c>
       <c r="E20" t="n">
-        <v>-51</v>
+        <v>-239</v>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>https://washingtoncitypaper.com/article/767013/needle-noem-dark-money-trump-musk/</t>
+          <t>https://washingtoncitypaper.com/article/775132/the-needle-costco-sues-over-tariffs-national-guard-member-shot-in-d-c-shows-positive-signs-and-trump-pardons-convicted-drug-trafficker/</t>
         </is>
       </c>
       <c r="G20" t="n">
-        <v>-49</v>
+        <v>-240</v>
       </c>
     </row>
     <row r="21">
@@ -949,24 +949,24 @@
         <v>0</v>
       </c>
       <c r="B21" t="n">
-        <v>76</v>
+        <v>144</v>
       </c>
       <c r="C21" s="2" t="n">
-        <v>45838</v>
+        <v>45992</v>
       </c>
       <c r="D21" t="n">
-        <v>-3</v>
+        <v>-9</v>
       </c>
       <c r="E21" t="n">
-        <v>-49</v>
+        <v>-240</v>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>https://washingtoncitypaper.com/article/766916/the-needle-the-supreme-court-continues-to-target-trans-rights-and-shady-doge-dealings/</t>
+          <t>https://washingtoncitypaper.com/article/774973/the-needle-rahmanullah-lakanwal-charged-with-murder-500-more-guard-members-to-join-the-2000-already-deployed-in-d-c-possible-war-crimes-and-business-isnt-booming-d-c/</t>
         </is>
       </c>
       <c r="G21" t="n">
-        <v>-46</v>
+        <v>-231</v>
       </c>
     </row>
     <row r="22">
@@ -974,24 +974,24 @@
         <v>0</v>
       </c>
       <c r="B22" t="n">
-        <v>75</v>
+        <v>143</v>
       </c>
       <c r="C22" s="2" t="n">
-        <v>45835</v>
+        <v>45987</v>
       </c>
       <c r="D22" t="n">
-        <v>-7</v>
+        <v>-4</v>
       </c>
       <c r="E22" t="n">
-        <v>-46</v>
+        <v>-231</v>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>https://washingtoncitypaper.com/article/766858/the-needle-a-series-of-blows-from-the-supreme-court/</t>
+          <t>https://washingtoncitypaper.com/article/774906/the-needle-doj-complaint-against-judge-dismissed-ice-wrongly-deported-trans-woman-and-former-death-row-prisoners-face-further-punishment-under-trump/</t>
         </is>
       </c>
       <c r="G22" t="n">
-        <v>-39</v>
+        <v>-228</v>
       </c>
     </row>
     <row r="23">
@@ -999,24 +999,24 @@
         <v>0</v>
       </c>
       <c r="B23" t="n">
-        <v>74</v>
+        <v>142</v>
       </c>
       <c r="C23" s="2" t="n">
-        <v>45834</v>
+        <v>45985</v>
       </c>
       <c r="D23" t="n">
-        <v>-7</v>
+        <v>-1</v>
       </c>
       <c r="E23" t="n">
-        <v>-39</v>
+        <v>-228</v>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>https://washingtoncitypaper.com/article/766793/the-needle-for-june-26/</t>
+          <t>https://washingtoncitypaper.com/article/774730/needle-indictment-redos-thousands-call-trump-impeachment-pardons-for-sale/</t>
         </is>
       </c>
       <c r="G23" t="n">
-        <v>-32</v>
+        <v>-227</v>
       </c>
     </row>
     <row r="24">
@@ -1024,24 +1024,24 @@
         <v>0</v>
       </c>
       <c r="B24" t="n">
-        <v>73</v>
+        <v>141</v>
       </c>
       <c r="C24" s="2" t="n">
-        <v>45833</v>
+        <v>45982</v>
       </c>
       <c r="D24" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="E24" t="n">
-        <v>-32</v>
+        <v>-227</v>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>https://washingtoncitypaper.com/article/766683/needle-iran-nuclear-facilities-attorneysgeneral-trump/</t>
+          <t>https://washingtoncitypaper.com/article/774683/needle-national-guard-in-d-c-illegal-police-shootings-hidden-in-secrecy/</t>
         </is>
       </c>
       <c r="G24" t="n">
-        <v>-31</v>
+        <v>-228</v>
       </c>
     </row>
     <row r="25">
@@ -1049,24 +1049,24 @@
         <v>0</v>
       </c>
       <c r="B25" t="n">
-        <v>72</v>
+        <v>140</v>
       </c>
       <c r="C25" s="2" t="n">
-        <v>45832</v>
+        <v>45981</v>
       </c>
       <c r="D25" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E25" t="n">
-        <v>-31</v>
+        <v>-228</v>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>https://washingtoncitypaper.com/article/766604/needle-elected-noncitizens-ceasefire/</t>
+          <t>https://washingtoncitypaper.com/article/774631/the-needle-house-passes-two-more-anti-d-c-bills-lawsuit-challenges-warrantless-arrests-of-migrants-and-alaska-national-guard-coming-to-d-c/</t>
         </is>
       </c>
       <c r="G25" t="n">
-        <v>-34</v>
+        <v>-228</v>
       </c>
     </row>
     <row r="26">
@@ -1074,24 +1074,24 @@
         <v>0</v>
       </c>
       <c r="B26" t="n">
-        <v>71</v>
+        <v>139</v>
       </c>
       <c r="C26" s="2" t="n">
-        <v>45831</v>
+        <v>45980</v>
       </c>
       <c r="D26" t="n">
-        <v>-2</v>
+        <v>1</v>
       </c>
       <c r="E26" t="n">
-        <v>-34</v>
+        <v>-228</v>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>https://washingtoncitypaper.com/article/766556/needle-iran-gay-pride-kennedy-center-juneteenth/</t>
+          <t>https://washingtoncitypaper.com/article/774543/needle-things-happen-texas-judges-racist-redistricting-release-epstein-files/</t>
         </is>
       </c>
       <c r="G26" t="n">
-        <v>-32</v>
+        <v>-235</v>
       </c>
     </row>
     <row r="27">
@@ -1099,24 +1099,24 @@
         <v>0</v>
       </c>
       <c r="B27" t="n">
-        <v>70</v>
+        <v>138</v>
       </c>
       <c r="C27" s="2" t="n">
-        <v>45827</v>
+        <v>45979</v>
       </c>
       <c r="D27" t="n">
-        <v>-3</v>
+        <v>-6</v>
       </c>
       <c r="E27" t="n">
-        <v>-32</v>
+        <v>-235</v>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>https://washingtoncitypaper.com/article/766409/needle-virginia-family-self-deport-foreign-med-students/</t>
+          <t>https://washingtoncitypaper.com/article/774464/the-needle-house-to-vote-on-epstein-release-pardoned-j6er-accused-of-sex-abuse-of-two-minors-and-self-admitted-nazi-gets-new-job-in-the-trump-administration/</t>
         </is>
       </c>
       <c r="G27" t="n">
-        <v>-35</v>
+        <v>-229</v>
       </c>
     </row>
     <row r="28">
@@ -1124,24 +1124,24 @@
         <v>0</v>
       </c>
       <c r="B28" t="n">
-        <v>69</v>
+        <v>137</v>
       </c>
       <c r="C28" s="2" t="n">
-        <v>45826</v>
+        <v>45975</v>
       </c>
       <c r="D28" t="n">
-        <v>-6</v>
+        <v>5</v>
       </c>
       <c r="E28" t="n">
-        <v>-35</v>
+        <v>-229</v>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>https://washingtoncitypaper.com/article/766285/needle-truck-tank-pedestrian-trans-medical-care/</t>
+          <t>https://washingtoncitypaper.com/article/774310/needle-another-federal-agent-shot-dc-driver/</t>
         </is>
       </c>
       <c r="G28" t="n">
-        <v>-29</v>
+        <v>-234</v>
       </c>
     </row>
     <row r="29">
@@ -1149,24 +1149,24 @@
         <v>0</v>
       </c>
       <c r="B29" t="n">
-        <v>68</v>
+        <v>136</v>
       </c>
       <c r="C29" s="2" t="n">
-        <v>45825</v>
+        <v>45974</v>
       </c>
       <c r="D29" t="n">
-        <v>-3</v>
+        <v>-1</v>
       </c>
       <c r="E29" t="n">
-        <v>-29</v>
+        <v>-234</v>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>https://washingtoncitypaper.com/article/766210/needle-streets-army-dhs/</t>
+          <t>https://washingtoncitypaper.com/article/774221/the-needle-bowser-celebrated-crime-stats-with-susie-wiles-trump-pressures-house-republicans-over-epstein-files-and-bishops-rebuke-immigration-tactics/</t>
         </is>
       </c>
       <c r="G29" t="n">
-        <v>-26</v>
+        <v>-233</v>
       </c>
     </row>
     <row r="30">
@@ -1174,24 +1174,24 @@
         <v>0</v>
       </c>
       <c r="B30" t="n">
-        <v>67</v>
+        <v>135</v>
       </c>
       <c r="C30" s="2" t="n">
-        <v>45824</v>
+        <v>45973</v>
       </c>
       <c r="D30" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="E30" t="n">
-        <v>-26</v>
+        <v>-233</v>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>https://washingtoncitypaper.com/article/766172/needle-deportation-trump-protests-no-kings/</t>
+          <t>https://washingtoncitypaper.com/article/774133/the-needle-d-c-police-lieutenant-confirms-work-with-ice-released-epstein-emails-say-trump-knew-about-the-girls/</t>
         </is>
       </c>
       <c r="G30" t="n">
-        <v>-31</v>
+        <v>-235</v>
       </c>
     </row>
     <row r="31">
@@ -1199,24 +1199,24 @@
         <v>0</v>
       </c>
       <c r="B31" t="n">
-        <v>66</v>
+        <v>134</v>
       </c>
       <c r="C31" s="2" t="n">
-        <v>45821</v>
+        <v>45972</v>
       </c>
       <c r="D31" t="n">
-        <v>2</v>
+        <v>-9</v>
       </c>
       <c r="E31" t="n">
-        <v>-31</v>
+        <v>-235</v>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>https://washingtoncitypaper.com/article/766120/the-needle-sen-padilla-cuffed-for-asking-questions-moco-students-walk-out-house-passes-another-anti-d-c-bill/</t>
+          <t>https://washingtoncitypaper.com/article/774066/needle-trump-booed-commanders-pardon-power-abuse-military-strikes-boats-killing-six/</t>
         </is>
       </c>
       <c r="G31" t="n">
-        <v>-35</v>
+        <v>-274</v>
       </c>
     </row>
     <row r="32">
@@ -1224,24 +1224,24 @@
         <v>0</v>
       </c>
       <c r="B32" t="n">
-        <v>65</v>
+        <v>133</v>
       </c>
       <c r="C32" s="2" t="n">
-        <v>45819</v>
+        <v>45965</v>
       </c>
       <c r="D32" t="n">
-        <v>2</v>
+        <v>-7</v>
       </c>
       <c r="E32" t="n">
-        <v>-35</v>
+        <v>-274</v>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>https://washingtoncitypaper.com/article/765993/the-needle-house-passes-two-anti-d-c-bills-anti-trump-protests-planned-this-weekend-and-nj-rep-indicted/</t>
+          <t>https://washingtoncitypaper.com/article/773622/needle-usao-crisis-pirro-ballroom-donors-billions-contracts/</t>
         </is>
       </c>
       <c r="G32" t="n">
-        <v>-37</v>
+        <v>-267</v>
       </c>
     </row>
     <row r="33">
@@ -1249,24 +1249,24 @@
         <v>0</v>
       </c>
       <c r="B33" t="n">
-        <v>64</v>
+        <v>132</v>
       </c>
       <c r="C33" s="2" t="n">
-        <v>45818</v>
+        <v>45964</v>
       </c>
       <c r="D33" t="n">
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="E33" t="n">
-        <v>-37</v>
+        <v>-267</v>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>https://washingtoncitypaper.com/article/765889/needle-road-closures-parade-bondi/</t>
+          <t>https://washingtoncitypaper.com/article/773572/needle-park-police-more-officers-mount-pleasant-tps-astronomy/</t>
         </is>
       </c>
       <c r="G33" t="n">
-        <v>-37</v>
+        <v>-262</v>
       </c>
     </row>
     <row r="34">
@@ -1274,24 +1274,24 @@
         <v>0</v>
       </c>
       <c r="B34" t="n">
-        <v>63</v>
+        <v>131</v>
       </c>
       <c r="C34" s="2" t="n">
-        <v>45817</v>
+        <v>45961</v>
       </c>
       <c r="D34" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="E34" t="n">
-        <v>-37</v>
+        <v>-262</v>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>https://washingtoncitypaper.com/article/765873/needle-kilmar-virginia-ice-trump-musk/</t>
+          <t>https://washingtoncitypaper.com/article/773547/needle-immigration-bus-stops-kennedy-center-ticket-sales/</t>
         </is>
       </c>
       <c r="G34" t="n">
-        <v>-36</v>
+        <v>-234</v>
       </c>
     </row>
     <row r="35">
@@ -1299,24 +1299,24 @@
         <v>0</v>
       </c>
       <c r="B35" t="n">
-        <v>62</v>
+        <v>130</v>
       </c>
       <c r="C35" s="2" t="n">
-        <v>45814</v>
+        <v>45957</v>
       </c>
       <c r="D35" t="n">
-        <v>2</v>
+        <v>-7</v>
       </c>
       <c r="E35" t="n">
-        <v>-36</v>
+        <v>-234</v>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>https://washingtoncitypaper.com/article/765615/the-needle-the-end-of-the-trump-musk-bromance/</t>
+          <t>https://washingtoncitypaper.com/article/773224/needle-norton-scammed-snap-confederate-statue-returns/</t>
         </is>
       </c>
       <c r="G35" t="n">
-        <v>-38</v>
+        <v>-225</v>
       </c>
     </row>
     <row r="36">
@@ -1324,24 +1324,24 @@
         <v>0</v>
       </c>
       <c r="B36" t="n">
-        <v>61</v>
+        <v>129</v>
       </c>
       <c r="C36" s="2" t="n">
-        <v>45814</v>
+        <v>45953</v>
       </c>
       <c r="D36" t="n">
-        <v>1</v>
+        <v>-2</v>
       </c>
       <c r="E36" t="n">
-        <v>-38</v>
+        <v>-225</v>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>https://washingtoncitypaper.com/article/765558/the-needle-travel-ban-2-0-and-illegal-deportations/</t>
+          <t>https://washingtoncitypaper.com/article/773052/needle-trump-demolish-east-wing-star-wars-national-guard/</t>
         </is>
       </c>
       <c r="G36" t="n">
-        <v>-39</v>
+        <v>-223</v>
       </c>
     </row>
     <row r="37">
@@ -1349,24 +1349,24 @@
         <v>0</v>
       </c>
       <c r="B37" t="n">
-        <v>60</v>
+        <v>128</v>
       </c>
       <c r="C37" s="2" t="n">
-        <v>45812</v>
+        <v>45952</v>
       </c>
       <c r="D37" t="n">
-        <v>0</v>
+        <v>-6</v>
       </c>
       <c r="E37" t="n">
-        <v>-39</v>
+        <v>-223</v>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>https://washingtoncitypaper.com/article/765487/the-needle-butterworths-trans-health-care-prison-hegseth/</t>
+          <t>https://washingtoncitypaper.com/article/772996/the-needle-trump-says-hes-owed-230-million-and-the-white-house-employee-with-a-self-described-nazi-streak-withdraws-nomination-to-lead-the-office-of-special-counsel/</t>
         </is>
       </c>
       <c r="G37" t="n">
-        <v>-39</v>
+        <v>-217</v>
       </c>
     </row>
     <row r="38">
@@ -1374,24 +1374,24 @@
         <v>0</v>
       </c>
       <c r="B38" t="n">
-        <v>59</v>
+        <v>127</v>
       </c>
       <c r="C38" s="2" t="n">
-        <v>45811</v>
+        <v>45951</v>
       </c>
       <c r="D38" t="n">
-        <v>-3</v>
+        <v>-6</v>
       </c>
       <c r="E38" t="n">
-        <v>-39</v>
+        <v>-217</v>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>https://washingtoncitypaper.com/article/765245/the-needle-deportation-museum-latino/</t>
+          <t>https://washingtoncitypaper.com/article/772970/needle-jeanine-pirro-fail-trump-nominee-nazi-streak-ice-applicants-fat/</t>
         </is>
       </c>
       <c r="G38" t="n">
-        <v>-36</v>
+        <v>-211</v>
       </c>
     </row>
     <row r="39">
@@ -1399,24 +1399,24 @@
         <v>0</v>
       </c>
       <c r="B39" t="n">
-        <v>58</v>
+        <v>126</v>
       </c>
       <c r="C39" s="2" t="n">
-        <v>45810</v>
+        <v>45950</v>
       </c>
       <c r="D39" t="n">
-        <v>-6</v>
+        <v>-2</v>
       </c>
       <c r="E39" t="n">
-        <v>-36</v>
+        <v>-211</v>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>https://washingtoncitypaper.com/article/765132/needle-rubio-afterschool-anacostia-community-museum/</t>
+          <t>https://washingtoncitypaper.com/article/772906/needle-trump-accused-murder-innocent-fisherman-rubio-betrayed-ms-13-informants/</t>
         </is>
       </c>
       <c r="G39" t="n">
-        <v>-30</v>
+        <v>-209</v>
       </c>
     </row>
     <row r="40">
@@ -1424,24 +1424,24 @@
         <v>0</v>
       </c>
       <c r="B40" t="n">
-        <v>57</v>
+        <v>125</v>
       </c>
       <c r="C40" s="2" t="n">
-        <v>45807</v>
+        <v>45947</v>
       </c>
       <c r="D40" t="n">
         <v>-2</v>
       </c>
       <c r="E40" t="n">
-        <v>-30</v>
+        <v>-209</v>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>https://washingtoncitypaper.com/article/765048/needle-supreme-court-immigration-trump-train/</t>
+          <t>https://washingtoncitypaper.com/article/772794/needle-trump-no-kings-national-guard-kavanaugh-stops/</t>
         </is>
       </c>
       <c r="G40" t="n">
-        <v>-28</v>
+        <v>-207</v>
       </c>
     </row>
     <row r="41">
@@ -1449,24 +1449,24 @@
         <v>0</v>
       </c>
       <c r="B41" t="n">
-        <v>56</v>
+        <v>124</v>
       </c>
       <c r="C41" s="2" t="n">
-        <v>45806</v>
+        <v>45946</v>
       </c>
       <c r="D41" t="n">
-        <v>4</v>
+        <v>-7</v>
       </c>
       <c r="E41" t="n">
-        <v>-28</v>
+        <v>-207</v>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>https://washingtoncitypaper.com/article/764968/needle-tariff-trump-musk/</t>
+          <t>https://washingtoncitypaper.com/article/772737/needle-rubio-visas-speech-trump-canceling-funds-democrats-boo-zoo-canceled/</t>
         </is>
       </c>
       <c r="G41" t="n">
-        <v>-32</v>
+        <v>-200</v>
       </c>
     </row>
     <row r="42">
@@ -1474,24 +1474,24 @@
         <v>0</v>
       </c>
       <c r="B42" t="n">
-        <v>55</v>
+        <v>123</v>
       </c>
       <c r="C42" s="2" t="n">
-        <v>45805</v>
+        <v>45945</v>
       </c>
       <c r="D42" t="n">
-        <v>-2</v>
+        <v>-11</v>
       </c>
       <c r="E42" t="n">
-        <v>-32</v>
+        <v>-200</v>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>https://washingtoncitypaper.com/article/764845/the-needle-trump-rains-on-worldpride-pardons-rich-friends-and-loses-to-the-lawyers/</t>
+          <t>https://washingtoncitypaper.com/article/772586/needle-young-republicans-racist-texts-leaked-trump-killing-six-boat/</t>
         </is>
       </c>
       <c r="G42" t="n">
-        <v>-30</v>
+        <v>-189</v>
       </c>
     </row>
     <row r="43">
@@ -1499,24 +1499,24 @@
         <v>0</v>
       </c>
       <c r="B43" t="n">
-        <v>54</v>
+        <v>122</v>
       </c>
       <c r="C43" s="2" t="n">
-        <v>45804</v>
+        <v>45944</v>
       </c>
       <c r="D43" t="n">
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="E43" t="n">
-        <v>-30</v>
+        <v>-189</v>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>https://washingtoncitypaper.com/article/764720/needle-jan-6-pardon-npr-sues-trump/</t>
+          <t>https://washingtoncitypaper.com/article/772523/needle-trump-fired-4000-pam-bondi-death-penalty-carjacker/</t>
         </is>
       </c>
       <c r="G43" t="n">
-        <v>-28</v>
+        <v>-186</v>
       </c>
     </row>
     <row r="44">
@@ -1524,24 +1524,24 @@
         <v>0</v>
       </c>
       <c r="B44" t="n">
-        <v>53</v>
+        <v>121</v>
       </c>
       <c r="C44" s="2" t="n">
-        <v>45800</v>
+        <v>45938</v>
       </c>
       <c r="D44" t="n">
-        <v>-1</v>
+        <v>-6</v>
       </c>
       <c r="E44" t="n">
-        <v>-28</v>
+        <v>-186</v>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>https://washingtoncitypaper.com/article/764660/needle-spit-ed-martin-crypto/</t>
+          <t>https://washingtoncitypaper.com/article/772420/needle-trump-backpay-shutdown/</t>
         </is>
       </c>
       <c r="G44" t="n">
-        <v>-27</v>
+        <v>-180</v>
       </c>
     </row>
     <row r="45">
@@ -1549,24 +1549,24 @@
         <v>0</v>
       </c>
       <c r="B45" t="n">
-        <v>52</v>
+        <v>120</v>
       </c>
       <c r="C45" s="2" t="n">
-        <v>45799</v>
+        <v>45937</v>
       </c>
       <c r="D45" t="n">
-        <v>4</v>
+        <v>-4</v>
       </c>
       <c r="E45" t="n">
-        <v>-27</v>
+        <v>-180</v>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>https://washingtoncitypaper.com/article/764538/needle-oval-military-parade-south-africa/</t>
+          <t>https://washingtoncitypaper.com/article/772320/needle-construction-immigration-investigate-cop-dont-call-911/</t>
         </is>
       </c>
       <c r="G45" t="n">
-        <v>-31</v>
+        <v>-176</v>
       </c>
     </row>
     <row r="46">
@@ -1574,24 +1574,24 @@
         <v>0</v>
       </c>
       <c r="B46" t="n">
-        <v>51</v>
+        <v>119</v>
       </c>
       <c r="C46" s="2" t="n">
-        <v>45798</v>
+        <v>45936</v>
       </c>
       <c r="D46" t="n">
-        <v>-6</v>
+        <v>0</v>
       </c>
       <c r="E46" t="n">
-        <v>-31</v>
+        <v>-176</v>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>https://washingtoncitypaper.com/article/764398/needle-covid-habeas-corpus/</t>
+          <t>https://washingtoncitypaper.com/article/772218/the-needle-judge-halts-national-guard-deployment-to-oregon-russell-voughts-suburban-virginia-neighbors-dont-like-him-and-kilmar-abrego-garcia-claims-vindictive-prosecution/</t>
         </is>
       </c>
       <c r="G46" t="n">
-        <v>-25</v>
+        <v>-170</v>
       </c>
     </row>
     <row r="47">
@@ -1599,24 +1599,24 @@
         <v>0</v>
       </c>
       <c r="B47" t="n">
-        <v>50</v>
+        <v>118</v>
       </c>
       <c r="C47" s="2" t="n">
-        <v>45797</v>
+        <v>45932</v>
       </c>
       <c r="D47" t="n">
-        <v>-7</v>
+        <v>-4</v>
       </c>
       <c r="E47" t="n">
-        <v>-25</v>
+        <v>-170</v>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>https://washingtoncitypaper.com/article/764351/needle-trump-doj-supreme-court/</t>
+          <t>https://washingtoncitypaper.com/article/772022/the-needle-trump-uses-shutdown-to-harm-democratic-cities-d-c-used-as-training-ground-for-local-ice-enforcement-and-dept-of-ed-sends-shakedown-letters/</t>
         </is>
       </c>
       <c r="G47" t="n">
-        <v>-18</v>
+        <v>-166</v>
       </c>
     </row>
     <row r="48">
@@ -1624,24 +1624,24 @@
         <v>0</v>
       </c>
       <c r="B48" t="n">
-        <v>49</v>
+        <v>117</v>
       </c>
       <c r="C48" s="2" t="n">
-        <v>45796</v>
+        <v>45931</v>
       </c>
       <c r="D48" t="n">
-        <v>-3</v>
+        <v>-12</v>
       </c>
       <c r="E48" t="n">
-        <v>-18</v>
+        <v>-166</v>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>https://washingtoncitypaper.com/article/764310/needle-arts-trump-doj-food-bank/</t>
+          <t>https://washingtoncitypaper.com/article/771885/needle-trump-bigoted-ai-hegseth-wastes-time-children-died-medicine-delayed/</t>
         </is>
       </c>
       <c r="G48" t="n">
-        <v>-15</v>
+        <v>-154</v>
       </c>
     </row>
     <row r="49">
@@ -1649,24 +1649,24 @@
         <v>0</v>
       </c>
       <c r="B49" t="n">
-        <v>48</v>
+        <v>116</v>
       </c>
       <c r="C49" s="2" t="n">
-        <v>45793</v>
+        <v>45930</v>
       </c>
       <c r="D49" t="n">
-        <v>-2</v>
+        <v>-9</v>
       </c>
       <c r="E49" t="n">
-        <v>-15</v>
+        <v>-154</v>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>https://washingtoncitypaper.com/article/764207/needle-kennedy-center-military-parade/</t>
+          <t>https://washingtoncitypaper.com/article/771817/the-needle-veteran-citizen-ice-shutdown-trump-racist-ai-video-alliance-healthcare/</t>
         </is>
       </c>
       <c r="G49" t="n">
-        <v>-13</v>
+        <v>-112</v>
       </c>
     </row>
     <row r="50">
@@ -1674,24 +1674,24 @@
         <v>0</v>
       </c>
       <c r="B50" t="n">
-        <v>47</v>
+        <v>115</v>
       </c>
       <c r="C50" s="2" t="n">
-        <v>45792</v>
+        <v>45922</v>
       </c>
       <c r="D50" t="n">
-        <v>1</v>
+        <v>-7</v>
       </c>
       <c r="E50" t="n">
-        <v>-13</v>
+        <v>-112</v>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>https://washingtoncitypaper.com/article/764120/needle-georgetown-student-protest-military-parade/</t>
+          <t>https://washingtoncitypaper.com/article/771302/needle-trump-bondi-enemies-tom-homan-bribery-stephen-miller-sidewalk-chalk/</t>
         </is>
       </c>
       <c r="G50" t="n">
-        <v>-14</v>
+        <v>-105</v>
       </c>
     </row>
     <row r="51">
@@ -1699,24 +1699,24 @@
         <v>0</v>
       </c>
       <c r="B51" t="n">
-        <v>46</v>
+        <v>114</v>
       </c>
       <c r="C51" s="2" t="n">
-        <v>45791</v>
+        <v>45919</v>
       </c>
       <c r="D51" t="n">
-        <v>-2</v>
+        <v>-9</v>
       </c>
       <c r="E51" t="n">
-        <v>-14</v>
+        <v>-105</v>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>https://washingtoncitypaper.com/article/764040/needle-trump-rich-undocumented/</t>
+          <t>https://washingtoncitypaper.com/article/771222/needle-robert-white-challenge-eleanor-neo-nazis-recruit/</t>
         </is>
       </c>
       <c r="G51" t="n">
-        <v>-12</v>
+        <v>-83</v>
       </c>
     </row>
     <row r="52">
@@ -1724,24 +1724,24 @@
         <v>0</v>
       </c>
       <c r="B52" t="n">
-        <v>45</v>
+        <v>113</v>
       </c>
       <c r="C52" s="2" t="n">
-        <v>45790</v>
+        <v>45915</v>
       </c>
       <c r="D52" t="n">
-        <v>-4</v>
+        <v>-7</v>
       </c>
       <c r="E52" t="n">
-        <v>-12</v>
+        <v>-83</v>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>https://washingtoncitypaper.com/article/763944/needle-plane-trump-lawyer/</t>
+          <t>https://washingtoncitypaper.com/article/770771/needle-trump-takeover-ice-killed-chicago-washington-post-fired-columnist/</t>
         </is>
       </c>
       <c r="G52" t="n">
-        <v>-8</v>
+        <v>-70</v>
       </c>
     </row>
     <row r="53">
@@ -1749,24 +1749,24 @@
         <v>0</v>
       </c>
       <c r="B53" t="n">
-        <v>44</v>
+        <v>112</v>
       </c>
       <c r="C53" s="2" t="n">
-        <v>45789</v>
+        <v>45911</v>
       </c>
       <c r="D53" t="n">
-        <v>-5</v>
+        <v>-8</v>
       </c>
       <c r="E53" t="n">
-        <v>-8</v>
+        <v>-70</v>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>https://washingtoncitypaper.com/article/763841/the-needle-a-flying-palace-trump-fam-profits-off-crypto-and-ed-martin-fails-up/</t>
+          <t>https://washingtoncitypaper.com/article/770576/needle-charlie-kirk-norton-home-rule-attacks-ice-arrests/</t>
         </is>
       </c>
       <c r="G53" t="n">
-        <v>-3</v>
+        <v>-62</v>
       </c>
     </row>
     <row r="54">
@@ -1774,24 +1774,24 @@
         <v>0</v>
       </c>
       <c r="B54" t="n">
-        <v>43</v>
+        <v>111</v>
       </c>
       <c r="C54" s="2" t="n">
-        <v>45786</v>
+        <v>45910</v>
       </c>
       <c r="D54" t="n">
-        <v>-3</v>
+        <v>-1</v>
       </c>
       <c r="E54" t="n">
-        <v>-3</v>
+        <v>-62</v>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>https://washingtoncitypaper.com/article/763748/needle-fired-feds-pentagon-trans-ban-carla-hayden/</t>
+          <t>https://washingtoncitypaper.com/article/770441/needle-dinner-trump-comparisons-hitler-immigration-arrests-dining/</t>
         </is>
       </c>
       <c r="G54" t="n">
-        <v>0</v>
+        <v>-61</v>
       </c>
     </row>
     <row r="55">
@@ -1799,24 +1799,24 @@
         <v>0</v>
       </c>
       <c r="B55" t="n">
-        <v>42</v>
+        <v>110</v>
       </c>
       <c r="C55" s="2" t="n">
-        <v>45785</v>
+        <v>45909</v>
       </c>
       <c r="D55" t="n">
-        <v>12</v>
+        <v>78</v>
       </c>
       <c r="E55" t="n">
-        <v>0</v>
+        <v>-61</v>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>https://washingtoncitypaper.com/article/763697/needle-ed-martin-les-mis-cast/</t>
+          <t>https://washingtoncitypaper.com/article/770375/needle-supreme-court-racial-discrimination-ice-trump-bday-card/</t>
         </is>
       </c>
       <c r="G55" t="n">
-        <v>-12</v>
+        <v>-139</v>
       </c>
     </row>
     <row r="56">
@@ -1824,24 +1824,24 @@
         <v>0</v>
       </c>
       <c r="B56" t="n">
-        <v>41</v>
+        <v>109</v>
       </c>
       <c r="C56" s="2" t="n">
-        <v>45784</v>
+        <v>45908</v>
       </c>
       <c r="D56" t="n">
         <v>-3</v>
       </c>
       <c r="E56" t="n">
-        <v>-12</v>
+        <v>-139</v>
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>https://washingtoncitypaper.com/article/763544/needle-supreme-trans-immigration-restaurants/</t>
+          <t>https://washingtoncitypaper.com/article/770322/needle-peace-vigil-trump-booed-us-open/</t>
         </is>
       </c>
       <c r="G56" t="n">
-        <v>-9</v>
+        <v>-136</v>
       </c>
     </row>
     <row r="57">
@@ -1849,24 +1849,24 @@
         <v>0</v>
       </c>
       <c r="B57" t="n">
-        <v>40</v>
+        <v>108</v>
       </c>
       <c r="C57" s="2" t="n">
-        <v>45783</v>
+        <v>45905</v>
       </c>
       <c r="D57" t="n">
-        <v>4</v>
+        <v>-1</v>
       </c>
       <c r="E57" t="n">
-        <v>-9</v>
+        <v>-136</v>
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>https://washingtoncitypaper.com/article/763500/needle-deportation-dc-budget-ed-martin/</t>
+          <t>https://washingtoncitypaper.com/article/770254/the-needle-stephen-miller-is-the-key-architect-of-trumps-federal-takeover-of-d-c-rfk-jr-lies-to-congress-and-magistrate-judge-slams-doj/</t>
         </is>
       </c>
       <c r="G57" t="n">
-        <v>-13</v>
+        <v>-135</v>
       </c>
     </row>
     <row r="58">
@@ -1874,24 +1874,24 @@
         <v>0</v>
       </c>
       <c r="B58" t="n">
-        <v>39</v>
+        <v>107</v>
       </c>
       <c r="C58" s="2" t="n">
-        <v>45782</v>
+        <v>45904</v>
       </c>
       <c r="D58" t="n">
         <v>2</v>
       </c>
       <c r="E58" t="n">
-        <v>-13</v>
+        <v>-135</v>
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>https://washingtoncitypaper.com/article/763437/needle-trump-business-deal-ethics-constitution/</t>
+          <t>https://washingtoncitypaper.com/article/770203/the-needle-d-c-national-guard-could-be-here-through-2025-a-g-schwalbs-lawsuit-calls-it-an-involuntary-military-occupation/</t>
         </is>
       </c>
       <c r="G58" t="n">
-        <v>-15</v>
+        <v>-134</v>
       </c>
     </row>
     <row r="59">
@@ -1899,24 +1899,24 @@
         <v>0</v>
       </c>
       <c r="B59" t="n">
-        <v>38</v>
+        <v>106</v>
       </c>
       <c r="C59" s="2" t="n">
-        <v>45779</v>
+        <v>45902</v>
       </c>
       <c r="D59" t="n">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="E59" t="n">
-        <v>-15</v>
+        <v>-134</v>
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>https://washingtoncitypaper.com/article/763378/needle-ed-martin-deportations-doge/</t>
+          <t>https://washingtoncitypaper.com/article/770078/the-needle-arlington-public-schools-challenges-the-department-of-education-and-kids-saved-from-deportation/</t>
         </is>
       </c>
       <c r="G59" t="n">
-        <v>-27</v>
+        <v>-134</v>
       </c>
     </row>
     <row r="60">
@@ -1924,24 +1924,24 @@
         <v>0</v>
       </c>
       <c r="B60" t="n">
-        <v>37</v>
+        <v>105</v>
       </c>
       <c r="C60" s="2" t="n">
-        <v>45778</v>
+        <v>45896</v>
       </c>
       <c r="D60" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E60" t="n">
-        <v>-27</v>
+        <v>-134</v>
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>https://washingtoncitypaper.com/article/763329/needle-journalists-may-day-protests/</t>
+          <t>https://washingtoncitypaper.com/article/769833/needle-trump-death-penalty-jeanine-pirro-indict-sandwich-thrower/</t>
         </is>
       </c>
       <c r="G60" t="n">
-        <v>-29</v>
+        <v>-129</v>
       </c>
     </row>
     <row r="61">
@@ -1949,24 +1949,24 @@
         <v>0</v>
       </c>
       <c r="B61" t="n">
-        <v>36</v>
+        <v>104</v>
       </c>
       <c r="C61" s="2" t="n">
-        <v>45777</v>
+        <v>45891</v>
       </c>
       <c r="D61" t="n">
-        <v>-5</v>
+        <v>-2</v>
       </c>
       <c r="E61" t="n">
-        <v>-29</v>
+        <v>-129</v>
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>https://washingtoncitypaper.com/article/763223/needle-trump-kilmar-republicans-medicaid/</t>
+          <t>https://washingtoncitypaper.com/article/769656/needle-chief-smith-mia-military-occupation-cost-1-million-per-day/</t>
         </is>
       </c>
       <c r="G61" t="n">
-        <v>-24</v>
+        <v>-127</v>
       </c>
     </row>
     <row r="62">
@@ -1974,24 +1974,24 @@
         <v>0</v>
       </c>
       <c r="B62" t="n">
-        <v>35</v>
+        <v>103</v>
       </c>
       <c r="C62" s="2" t="n">
-        <v>45776</v>
+        <v>45890</v>
       </c>
       <c r="D62" t="n">
-        <v>-5</v>
+        <v>-6</v>
       </c>
       <c r="E62" t="n">
-        <v>-24</v>
+        <v>-127</v>
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>https://washingtoncitypaper.com/article/763129/needle-ed-martin-nazi/</t>
+          <t>https://washingtoncitypaper.com/article/769599/needlemilitary-vehicle-crash-vance-booed-union-station/</t>
         </is>
       </c>
       <c r="G62" t="n">
-        <v>-19</v>
+        <v>-121</v>
       </c>
     </row>
     <row r="63">
@@ -1999,24 +1999,24 @@
         <v>0</v>
       </c>
       <c r="B63" t="n">
-        <v>34</v>
+        <v>102</v>
       </c>
       <c r="C63" s="2" t="n">
-        <v>45775</v>
+        <v>45889</v>
       </c>
       <c r="D63" t="n">
-        <v>2</v>
+        <v>-9</v>
       </c>
       <c r="E63" t="n">
-        <v>-19</v>
+        <v>-121</v>
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>https://washingtoncitypaper.com/article/763081/the-needle-99-days-of-trump/</t>
+          <t>https://washingtoncitypaper.com/article/769491/the-needle-the-smithsonian-is-too-woke-hate-speech-from-a-speech-writer-and-secret-police-terrorize-d-c/</t>
         </is>
       </c>
       <c r="G63" t="n">
-        <v>-15</v>
+        <v>-118</v>
       </c>
     </row>
     <row r="64">
@@ -2024,24 +2024,24 @@
         <v>0</v>
       </c>
       <c r="B64" t="n">
-        <v>33</v>
+        <v>101</v>
       </c>
       <c r="C64" s="2" t="n">
-        <v>45771</v>
+        <v>45888</v>
       </c>
       <c r="D64" t="n">
-        <v>-3</v>
+        <v>-4</v>
       </c>
       <c r="E64" t="n">
-        <v>-15</v>
+        <v>-118</v>
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>https://washingtoncitypaper.com/article/762919/needle-ed-martin-abrego-garcia-smithsonian/</t>
+          <t>https://washingtoncitypaper.com/article/769455/the-needle-three-more-states-to-send-national-guards-to-d-c-and-five-virginia-school-districts-refuse-to-rescind-trans-affirming-policies/</t>
         </is>
       </c>
       <c r="G64" t="n">
-        <v>-12</v>
+        <v>-114</v>
       </c>
     </row>
     <row r="65">
@@ -2049,24 +2049,24 @@
         <v>0</v>
       </c>
       <c r="B65" t="n">
-        <v>32</v>
+        <v>100</v>
       </c>
       <c r="C65" s="2" t="n">
-        <v>45770</v>
+        <v>45887</v>
       </c>
       <c r="D65" t="n">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="E65" t="n">
-        <v>-12</v>
+        <v>-114</v>
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>https://washingtoncitypaper.com/article/762817/needle-ed-martin-lgbtqia-hhs/</t>
+          <t>https://washingtoncitypaper.com/article/769390/needle-mpd-takeover-immigration-enforcement/</t>
         </is>
       </c>
       <c r="G65" t="n">
-        <v>-11</v>
+        <v>-112</v>
       </c>
     </row>
     <row r="66">
@@ -2074,24 +2074,24 @@
         <v>0</v>
       </c>
       <c r="B66" t="n">
-        <v>31</v>
+        <v>99</v>
       </c>
       <c r="C66" s="2" t="n">
-        <v>45769</v>
+        <v>45883</v>
       </c>
       <c r="D66" t="n">
-        <v>-11</v>
+        <v>-9</v>
       </c>
       <c r="E66" t="n">
-        <v>-11</v>
+        <v>-112</v>
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>https://washingtoncitypaper.com/article/762704/needle-harvard-cancer-scientist/</t>
+          <t>https://washingtoncitypaper.com/article/769265/needle-trump-mpd-pamela-smith-takeover-subway/</t>
         </is>
       </c>
       <c r="G66" t="n">
-        <v>0</v>
+        <v>-103</v>
       </c>
     </row>
     <row r="67">
@@ -2099,24 +2099,24 @@
         <v>0</v>
       </c>
       <c r="B67" t="n">
-        <v>30</v>
+        <v>98</v>
       </c>
       <c r="C67" s="2" t="n">
-        <v>45768</v>
+        <v>45882</v>
       </c>
       <c r="D67" t="n">
-        <v>8</v>
+        <v>-5</v>
       </c>
       <c r="E67" t="n">
-        <v>0</v>
+        <v>-103</v>
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>https://washingtoncitypaper.com/article/762610/needle-hegseth-supremecourt-immigration-deportation/</t>
+          <t>https://washingtoncitypaper.com/article/769174/needle-smithsonian-confusion-mpd-homeless-jailed/</t>
         </is>
       </c>
       <c r="G67" t="n">
-        <v>-8</v>
+        <v>-98</v>
       </c>
     </row>
     <row r="68">
@@ -2124,24 +2124,24 @@
         <v>0</v>
       </c>
       <c r="B68" t="n">
-        <v>29</v>
+        <v>97</v>
       </c>
       <c r="C68" s="2" t="n">
-        <v>45765</v>
+        <v>45881</v>
       </c>
       <c r="D68" t="n">
-        <v>12</v>
+        <v>-3</v>
       </c>
       <c r="E68" t="n">
-        <v>-8</v>
+        <v>-98</v>
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>https://washingtoncitypaper.com/article/762539/needle-kilmar-vanhollen/</t>
+          <t>https://washingtoncitypaper.com/article/769131/needle-ag-forced-hospitalizations-black-church-proud-boys/</t>
         </is>
       </c>
       <c r="G68" t="n">
-        <v>-20</v>
+        <v>-94</v>
       </c>
     </row>
     <row r="69">
@@ -2149,24 +2149,24 @@
         <v>0</v>
       </c>
       <c r="B69" t="n">
-        <v>28</v>
+        <v>96</v>
       </c>
       <c r="C69" s="2" t="n">
-        <v>45764</v>
+        <v>45877</v>
       </c>
       <c r="D69" t="n">
-        <v>-3</v>
+        <v>-4</v>
       </c>
       <c r="E69" t="n">
-        <v>-20</v>
+        <v>-94</v>
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>https://washingtoncitypaper.com/article/762425/needle-van-hollen-harvard/</t>
+          <t>https://washingtoncitypaper.com/article/769029/the-needle-feds-patrolling-d-c-streets-pirro-calls-on-d-c-council-to-repeal-restorative-justice-laws-and-trans-air-force-members-lose-retirement-benefits/</t>
         </is>
       </c>
       <c r="G69" t="n">
-        <v>-8</v>
+        <v>-90</v>
       </c>
     </row>
     <row r="70">
@@ -2174,24 +2174,24 @@
         <v>0</v>
       </c>
       <c r="B70" t="n">
-        <v>27</v>
+        <v>95</v>
       </c>
       <c r="C70" s="2" t="n">
-        <v>45762</v>
+        <v>45876</v>
       </c>
       <c r="D70" t="n">
         <v>-2</v>
       </c>
       <c r="E70" t="n">
-        <v>-8</v>
+        <v>-90</v>
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>https://washingtoncitypaper.com/article/762198/needle-doge-data-nlrb-whistleblower/</t>
+          <t>https://washingtoncitypaper.com/article/768905/trumps-remaking-the-criminal-justice-system-and-14-states-plus-d-c-sue-for-gender-affirming-care/</t>
         </is>
       </c>
       <c r="G70" t="n">
-        <v>0</v>
+        <v>-88</v>
       </c>
     </row>
     <row r="71">
@@ -2199,24 +2199,24 @@
         <v>0</v>
       </c>
       <c r="B71" t="n">
-        <v>26</v>
+        <v>94</v>
       </c>
       <c r="C71" s="2" t="n">
-        <v>45758</v>
+        <v>45875</v>
       </c>
       <c r="D71" t="n">
-        <v>8</v>
+        <v>-6</v>
       </c>
       <c r="E71" t="n">
-        <v>0</v>
+        <v>-88</v>
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>https://washingtoncitypaper.com/article/762084/needle-abregogarcia-ice-rubio-eggs/</t>
+          <t>https://washingtoncitypaper.com/article/768849/needle-big-balls-assault-federal-takeover-family-separations/</t>
         </is>
       </c>
       <c r="G71" t="n">
-        <v>-5</v>
+        <v>-76</v>
       </c>
     </row>
     <row r="72">
@@ -2224,24 +2224,24 @@
         <v>0</v>
       </c>
       <c r="B72" t="n">
-        <v>25</v>
+        <v>93</v>
       </c>
       <c r="C72" s="2" t="n">
-        <v>45756</v>
+        <v>45869</v>
       </c>
       <c r="D72" t="n">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="E72" t="n">
-        <v>-5</v>
+        <v>-76</v>
       </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>https://washingtoncitypaper.com/article/762015/needle-press-pronouns-first-amendment/</t>
+          <t>https://washingtoncitypaper.com/article/768593/needle-social-security-epstein-layoffs-buyout-ice/</t>
         </is>
       </c>
       <c r="G72" t="n">
-        <v>-4</v>
+        <v>-74</v>
       </c>
     </row>
     <row r="73">
@@ -2249,24 +2249,24 @@
         <v>0</v>
       </c>
       <c r="B73" t="n">
-        <v>24</v>
+        <v>92</v>
       </c>
       <c r="C73" s="2" t="n">
-        <v>45755</v>
+        <v>45868</v>
       </c>
       <c r="D73" t="n">
-        <v>-5</v>
+        <v>-6</v>
       </c>
       <c r="E73" t="n">
-        <v>-4</v>
+        <v>-74</v>
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>https://washingtoncitypaper.com/article/761902/needle-negative-supreme-court/</t>
+          <t>https://washingtoncitypaper.com/article/768494/needle-pirro-status-check-bove-epa-climate-change/</t>
         </is>
       </c>
       <c r="G73" t="n">
-        <v>4</v>
+        <v>-68</v>
       </c>
     </row>
     <row r="74">
@@ -2274,24 +2274,24 @@
         <v>0</v>
       </c>
       <c r="B74" t="n">
-        <v>23</v>
+        <v>91</v>
       </c>
       <c r="C74" s="2" t="n">
-        <v>45751</v>
+        <v>45867</v>
       </c>
       <c r="D74" t="n">
-        <v>0</v>
+        <v>-3</v>
       </c>
       <c r="E74" t="n">
-        <v>4</v>
+        <v>-68</v>
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>https://washingtoncitypaper.com/article/761750/needle-laura-loomer-trump/</t>
+          <t>https://washingtoncitypaper.com/article/768423/the-needle-ices-masks-draw-imposters-another-whistleblower-accuses-bove-and-republicans-want-to-rename-the-kennedy-center/</t>
         </is>
       </c>
       <c r="G74" t="n">
-        <v>4</v>
+        <v>-65</v>
       </c>
     </row>
     <row r="75">
@@ -2299,24 +2299,24 @@
         <v>0</v>
       </c>
       <c r="B75" t="n">
-        <v>22</v>
+        <v>90</v>
       </c>
       <c r="C75" s="2" t="n">
-        <v>45750</v>
+        <v>45866</v>
       </c>
       <c r="D75" t="n">
-        <v>-5</v>
+        <v>-3</v>
       </c>
       <c r="E75" t="n">
-        <v>4</v>
+        <v>-65</v>
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>https://washingtoncitypaper.com/article/761656/needle-trade-war-budget/</t>
+          <t>https://washingtoncitypaper.com/article/768370/needle-scotland-troll-trump-qatar-jet-darren-beattie/</t>
         </is>
       </c>
       <c r="G75" t="n">
-        <v>9</v>
+        <v>-62</v>
       </c>
     </row>
     <row r="76">
@@ -2324,24 +2324,24 @@
         <v>0</v>
       </c>
       <c r="B76" t="n">
-        <v>21</v>
+        <v>89</v>
       </c>
       <c r="C76" s="2" t="n">
-        <v>45749</v>
+        <v>45863</v>
       </c>
       <c r="D76" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E76" t="n">
-        <v>9</v>
+        <v>-62</v>
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>https://washingtoncitypaper.com/article/761599/needle-booker-schiff-martin/</t>
+          <t>https://washingtoncitypaper.com/article/768303/needle-trump-republicans-oil-and-gas-companies-immigration-lawsuit/</t>
         </is>
       </c>
       <c r="G76" t="n">
-        <v>5</v>
+        <v>-62</v>
       </c>
     </row>
     <row r="77">
@@ -2349,24 +2349,24 @@
         <v>0</v>
       </c>
       <c r="B77" t="n">
-        <v>20</v>
+        <v>88</v>
       </c>
       <c r="C77" s="2" t="n">
-        <v>45748</v>
+        <v>45862</v>
       </c>
       <c r="D77" t="n">
-        <v>-5</v>
+        <v>-1</v>
       </c>
       <c r="E77" t="n">
-        <v>5</v>
+        <v>-62</v>
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>https://washingtoncitypaper.com/article/761505/needle-immigration-deportation-error/</t>
+          <t>https://washingtoncitypaper.com/article/768246/needle-weed-park-police-arrests/</t>
         </is>
       </c>
       <c r="G77" t="n">
-        <v>10</v>
+        <v>-61</v>
       </c>
     </row>
     <row r="78">
@@ -2374,24 +2374,24 @@
         <v>0</v>
       </c>
       <c r="B78" t="n">
-        <v>19</v>
+        <v>87</v>
       </c>
       <c r="C78" s="2" t="n">
-        <v>45747</v>
+        <v>45861</v>
       </c>
       <c r="D78" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E78" t="n">
-        <v>10</v>
+        <v>-61</v>
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>https://washingtoncitypaper.com/article/761408/needle-third-term/</t>
+          <t>https://washingtoncitypaper.com/article/768177/needle-ice-kids-feds-capitol-hill/</t>
         </is>
       </c>
       <c r="G78" t="n">
-        <v>10</v>
+        <v>-66</v>
       </c>
     </row>
     <row r="79">
@@ -2399,24 +2399,24 @@
         <v>0</v>
       </c>
       <c r="B79" t="n">
-        <v>18</v>
+        <v>86</v>
       </c>
       <c r="C79" s="2" t="n">
-        <v>45744</v>
+        <v>45860</v>
       </c>
       <c r="D79" t="n">
-        <v>-12</v>
+        <v>-3</v>
       </c>
       <c r="E79" t="n">
-        <v>10</v>
+        <v>-66</v>
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>https://washingtoncitypaper.com/article/761339/needle-trump-executive-order-public-safety/</t>
+          <t>https://washingtoncitypaper.com/article/768121/needle-trump-distract-epstein/</t>
         </is>
       </c>
       <c r="G79" t="n">
-        <v>22</v>
+        <v>-63</v>
       </c>
     </row>
     <row r="80">
@@ -2424,24 +2424,24 @@
         <v>0</v>
       </c>
       <c r="B80" t="n">
-        <v>17</v>
+        <v>85</v>
       </c>
       <c r="C80" s="2" t="n">
-        <v>45743</v>
+        <v>45859</v>
       </c>
       <c r="D80" t="n">
-        <v>1</v>
+        <v>-2</v>
       </c>
       <c r="E80" t="n">
-        <v>22</v>
+        <v>-63</v>
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>https://washingtoncitypaper.com/article/761265/needle-judge-boasberg-hdcooke-signal/</t>
+          <t>https://washingtoncitypaper.com/article/768062/the-needle-trump-says-rename-the-commanders-or-else-and-the-presidents-history-of-doodling/</t>
         </is>
       </c>
       <c r="G80" t="n">
-        <v>21</v>
+        <v>-61</v>
       </c>
     </row>
     <row r="81">
@@ -2449,24 +2449,24 @@
         <v>0</v>
       </c>
       <c r="B81" t="n">
-        <v>16</v>
+        <v>84</v>
       </c>
       <c r="C81" s="2" t="n">
-        <v>45742</v>
+        <v>45856</v>
       </c>
       <c r="D81" t="n">
         <v>-5</v>
       </c>
       <c r="E81" t="n">
-        <v>21</v>
+        <v>-61</v>
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>https://washingtoncitypaper.com/article/761141/the-needle-district-of-america-edition/</t>
+          <t>https://washingtoncitypaper.com/article/768013/the-needle-lgbtqia-youth-hotline-is-disconnected-and-ice-gets-access-to-medicaid-records/</t>
         </is>
       </c>
       <c r="G81" t="n">
-        <v>26</v>
+        <v>-56</v>
       </c>
     </row>
     <row r="82">
@@ -2474,24 +2474,24 @@
         <v>0</v>
       </c>
       <c r="B82" t="n">
-        <v>15</v>
+        <v>83</v>
       </c>
       <c r="C82" s="2" t="n">
-        <v>45741</v>
+        <v>45855</v>
       </c>
       <c r="D82" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="E82" t="n">
-        <v>26</v>
+        <v>-56</v>
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>https://washingtoncitypaper.com/article/761005/the-needle-group-chat-edition/</t>
+          <t>https://washingtoncitypaper.com/article/767964/the-needle-protest-civil-rights-rollback-convention-industry-hit/</t>
         </is>
       </c>
       <c r="G82" t="n">
-        <v>26</v>
+        <v>-55</v>
       </c>
     </row>
     <row r="83">
@@ -2499,24 +2499,24 @@
         <v>0</v>
       </c>
       <c r="B83" t="n">
-        <v>14</v>
+        <v>82</v>
       </c>
       <c r="C83" s="2" t="n">
-        <v>45740</v>
+        <v>45854</v>
       </c>
       <c r="D83" t="n">
-        <v>-4</v>
+        <v>1</v>
       </c>
       <c r="E83" t="n">
-        <v>26</v>
+        <v>-55</v>
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>https://washingtoncitypaper.com/article/760917/needle-musk-ed-martin/</t>
+          <t>https://washingtoncitypaper.com/article/767861/needle-inflation-speaker-johnson-epstein-protest/</t>
         </is>
       </c>
       <c r="G83" t="n">
-        <v>30</v>
+        <v>-56</v>
       </c>
     </row>
     <row r="84">
@@ -2524,24 +2524,24 @@
         <v>0</v>
       </c>
       <c r="B84" t="n">
-        <v>13</v>
+        <v>81</v>
       </c>
       <c r="C84" s="2" t="n">
-        <v>45737</v>
+        <v>45853</v>
       </c>
       <c r="D84" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="E84" t="n">
-        <v>30</v>
+        <v>-56</v>
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>https://washingtoncitypaper.com/article/760826/needle-trump-musk-deportation-immigrant-georgetown/</t>
+          <t>https://washingtoncitypaper.com/article/767762/needle-detained-migrants-maga-epstein-education-department/</t>
         </is>
       </c>
       <c r="G84" t="n">
-        <v>31</v>
+        <v>-57</v>
       </c>
     </row>
     <row r="85">
@@ -2549,24 +2549,24 @@
         <v>0</v>
       </c>
       <c r="B85" t="n">
-        <v>12</v>
+        <v>80</v>
       </c>
       <c r="C85" s="2" t="n">
-        <v>45736</v>
+        <v>45852</v>
       </c>
       <c r="D85" t="n">
-        <v>-3</v>
+        <v>0</v>
       </c>
       <c r="E85" t="n">
-        <v>31</v>
+        <v>-57</v>
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>https://washingtoncitypaper.com/article/760736/needle-georgetown-immigration-tarrio/</t>
+          <t>https://washingtoncitypaper.com/article/767708/the-needle-usao-spokesperson-fired-trump-booed-in-jersey-and-rosie-odonnell-claps-back/</t>
         </is>
       </c>
       <c r="G85" t="n">
-        <v>34</v>
+        <v>-63</v>
       </c>
     </row>
     <row r="86">
@@ -2574,24 +2574,24 @@
         <v>0</v>
       </c>
       <c r="B86" t="n">
-        <v>11</v>
+        <v>79</v>
       </c>
       <c r="C86" s="2" t="n">
-        <v>45735</v>
+        <v>45848</v>
       </c>
       <c r="D86" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="E86" t="n">
-        <v>34</v>
+        <v>-63</v>
       </c>
       <c r="F86" t="inlineStr">
         <is>
-          <t>https://washingtoncitypaper.com/article/760643/the-needle-judgment-day-edition/</t>
+          <t>https://washingtoncitypaper.com/article/767546/needle-trump-english-liberia-research/</t>
         </is>
       </c>
       <c r="G86" t="n">
-        <v>35</v>
+        <v>-61</v>
       </c>
     </row>
     <row r="87">
@@ -2599,24 +2599,24 @@
         <v>0</v>
       </c>
       <c r="B87" t="n">
-        <v>10</v>
+        <v>78</v>
       </c>
       <c r="C87" s="2" t="n">
-        <v>45734</v>
+        <v>45845</v>
       </c>
       <c r="D87" t="n">
-        <v>1</v>
+        <v>-4</v>
       </c>
       <c r="E87" t="n">
-        <v>35</v>
+        <v>-61</v>
       </c>
       <c r="F87" t="inlineStr">
         <is>
-          <t>https://washingtoncitypaper.com/article/760572/needle-semisonic-kennedy-center-trump/</t>
+          <t>https://washingtoncitypaper.com/article/767316/the-needle-tens-of-thousands-in-d-c-will-lose-health-coverage-under-trumps-big-bill/</t>
         </is>
       </c>
       <c r="G87" t="n">
-        <v>34</v>
+        <v>-54</v>
       </c>
     </row>
     <row r="88">
@@ -2624,24 +2624,24 @@
         <v>0</v>
       </c>
       <c r="B88" t="n">
-        <v>9</v>
+        <v>77</v>
       </c>
       <c r="C88" s="2" t="n">
-        <v>45733</v>
+        <v>45840</v>
       </c>
       <c r="D88" t="n">
-        <v>-5</v>
+        <v>-3</v>
       </c>
       <c r="E88" t="n">
-        <v>34</v>
+        <v>-54</v>
       </c>
       <c r="F88" t="inlineStr">
         <is>
-          <t>https://washingtoncitypaper.com/article/760471/the-needle-deportation-budget/</t>
+          <t>https://washingtoncitypaper.com/article/767067/needle-health-insurance-senate-anacostia-community-museum/</t>
         </is>
       </c>
       <c r="G88" t="n">
-        <v>39</v>
+        <v>-51</v>
       </c>
     </row>
     <row r="89">
@@ -2649,24 +2649,24 @@
         <v>0</v>
       </c>
       <c r="B89" t="n">
-        <v>8</v>
+        <v>76</v>
       </c>
       <c r="C89" s="2" t="n">
-        <v>45730</v>
+        <v>45839</v>
       </c>
       <c r="D89" t="n">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="E89" t="n">
-        <v>39</v>
+        <v>-51</v>
       </c>
       <c r="F89" t="inlineStr">
         <is>
-          <t>https://washingtoncitypaper.com/article/760390/needle-ed-martin-jd-vance-budget/</t>
+          <t>https://washingtoncitypaper.com/article/767013/needle-noem-dark-money-trump-musk/</t>
         </is>
       </c>
       <c r="G89" t="n">
-        <v>39</v>
+        <v>-49</v>
       </c>
     </row>
     <row r="90">
@@ -2674,24 +2674,24 @@
         <v>0</v>
       </c>
       <c r="B90" t="n">
-        <v>7</v>
+        <v>75</v>
       </c>
       <c r="C90" s="2" t="n">
-        <v>45729</v>
+        <v>45838</v>
       </c>
       <c r="D90" t="n">
-        <v>2</v>
+        <v>-3</v>
       </c>
       <c r="E90" t="n">
-        <v>39</v>
+        <v>-49</v>
       </c>
       <c r="F90" t="inlineStr">
         <is>
-          <t>https://washingtoncitypaper.com/article/760275/the-needle-musk-doge-budget/</t>
+          <t>https://washingtoncitypaper.com/article/766916/the-needle-the-supreme-court-continues-to-target-trans-rights-and-shady-doge-dealings/</t>
         </is>
       </c>
       <c r="G90" t="n">
-        <v>37</v>
+        <v>-46</v>
       </c>
     </row>
     <row r="91">
@@ -2699,24 +2699,24 @@
         <v>0</v>
       </c>
       <c r="B91" t="n">
-        <v>6</v>
+        <v>74</v>
       </c>
       <c r="C91" s="2" t="n">
-        <v>45728</v>
+        <v>45835</v>
       </c>
       <c r="D91" t="n">
-        <v>-9</v>
+        <v>-7</v>
       </c>
       <c r="E91" t="n">
-        <v>37</v>
+        <v>-46</v>
       </c>
       <c r="F91" t="inlineStr">
         <is>
-          <t>https://washingtoncitypaper.com/article/760149/the-needle-retribution-watch-edition/</t>
+          <t>https://washingtoncitypaper.com/article/766858/the-needle-a-series-of-blows-from-the-supreme-court/</t>
         </is>
       </c>
       <c r="G91" t="n">
-        <v>37</v>
+        <v>-39</v>
       </c>
     </row>
     <row r="92">
@@ -2724,24 +2724,24 @@
         <v>0</v>
       </c>
       <c r="B92" t="n">
-        <v>5</v>
+        <v>73</v>
       </c>
       <c r="C92" s="2" t="n">
-        <v>45728</v>
+        <v>45834</v>
       </c>
       <c r="D92" t="n">
-        <v>-9</v>
+        <v>-7</v>
       </c>
       <c r="E92" t="n">
-        <v>37</v>
+        <v>-39</v>
       </c>
       <c r="F92" t="inlineStr">
         <is>
-          <t>https://washingtoncitypaper.com/article/760149/the-needle-retribution-watch-edition/</t>
+          <t>https://washingtoncitypaper.com/article/766793/the-needle-for-june-26/</t>
         </is>
       </c>
       <c r="G92" t="n">
-        <v>46</v>
+        <v>-32</v>
       </c>
     </row>
     <row r="93">
@@ -2749,24 +2749,24 @@
         <v>0</v>
       </c>
       <c r="B93" t="n">
-        <v>4</v>
+        <v>72</v>
       </c>
       <c r="C93" s="2" t="n">
-        <v>45727</v>
+        <v>45833</v>
       </c>
       <c r="D93" t="n">
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="E93" t="n">
-        <v>46</v>
+        <v>-32</v>
       </c>
       <c r="F93" t="inlineStr">
         <is>
-          <t>https://washingtoncitypaper.com/article/760018/needle-budget-jobs/</t>
+          <t>https://washingtoncitypaper.com/article/766683/needle-iran-nuclear-facilities-attorneysgeneral-trump/</t>
         </is>
       </c>
       <c r="G93" t="n">
-        <v>44</v>
+        <v>-31</v>
       </c>
     </row>
     <row r="94">
@@ -2774,24 +2774,24 @@
         <v>0</v>
       </c>
       <c r="B94" t="n">
+        <v>71</v>
+      </c>
+      <c r="C94" s="2" t="n">
+        <v>45832</v>
+      </c>
+      <c r="D94" t="n">
         <v>3</v>
       </c>
-      <c r="C94" s="2" t="n">
-        <v>45726</v>
-      </c>
-      <c r="D94" t="n">
-        <v>-13</v>
-      </c>
       <c r="E94" t="n">
-        <v>44</v>
+        <v>-31</v>
       </c>
       <c r="F94" t="inlineStr">
         <is>
-          <t>https://washingtoncitypaper.com/article/759853/the-needle-budget-blow-up-edition/</t>
+          <t>https://washingtoncitypaper.com/article/766604/needle-elected-noncitizens-ceasefire/</t>
         </is>
       </c>
       <c r="G94" t="n">
-        <v>57</v>
+        <v>-34</v>
       </c>
     </row>
     <row r="95">
@@ -2799,24 +2799,24 @@
         <v>0</v>
       </c>
       <c r="B95" t="n">
-        <v>2</v>
+        <v>70</v>
       </c>
       <c r="C95" s="2" t="n">
-        <v>45723</v>
+        <v>45831</v>
       </c>
       <c r="D95" t="n">
-        <v>-11</v>
+        <v>-2</v>
       </c>
       <c r="E95" t="n">
-        <v>57</v>
+        <v>-34</v>
       </c>
       <c r="F95" t="inlineStr">
         <is>
-          <t>https://washingtoncitypaper.com/article/759667/the-needle-capitulation-watch-edition/</t>
+          <t>https://washingtoncitypaper.com/article/766556/needle-iran-gay-pride-kennedy-center-juneteenth/</t>
         </is>
       </c>
       <c r="G95" t="n">
-        <v>68</v>
+        <v>-32</v>
       </c>
     </row>
     <row r="96">
@@ -2824,23 +2824,1723 @@
         <v>0</v>
       </c>
       <c r="B96" t="n">
+        <v>69</v>
+      </c>
+      <c r="C96" s="2" t="n">
+        <v>45827</v>
+      </c>
+      <c r="D96" t="n">
+        <v>-3</v>
+      </c>
+      <c r="E96" t="n">
+        <v>-32</v>
+      </c>
+      <c r="F96" t="inlineStr">
+        <is>
+          <t>https://washingtoncitypaper.com/article/766409/needle-virginia-family-self-deport-foreign-med-students/</t>
+        </is>
+      </c>
+      <c r="G96" t="n">
+        <v>-35</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B97" t="n">
+        <v>68</v>
+      </c>
+      <c r="C97" s="2" t="n">
+        <v>45826</v>
+      </c>
+      <c r="D97" t="n">
+        <v>-6</v>
+      </c>
+      <c r="E97" t="n">
+        <v>-35</v>
+      </c>
+      <c r="F97" t="inlineStr">
+        <is>
+          <t>https://washingtoncitypaper.com/article/766285/needle-truck-tank-pedestrian-trans-medical-care/</t>
+        </is>
+      </c>
+      <c r="G97" t="n">
+        <v>-29</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B98" t="n">
+        <v>67</v>
+      </c>
+      <c r="C98" s="2" t="n">
+        <v>45825</v>
+      </c>
+      <c r="D98" t="n">
+        <v>-3</v>
+      </c>
+      <c r="E98" t="n">
+        <v>-29</v>
+      </c>
+      <c r="F98" t="inlineStr">
+        <is>
+          <t>https://washingtoncitypaper.com/article/766210/needle-streets-army-dhs/</t>
+        </is>
+      </c>
+      <c r="G98" t="n">
+        <v>-26</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B99" t="n">
+        <v>66</v>
+      </c>
+      <c r="C99" s="2" t="n">
+        <v>45824</v>
+      </c>
+      <c r="D99" t="n">
+        <v>7</v>
+      </c>
+      <c r="E99" t="n">
+        <v>-26</v>
+      </c>
+      <c r="F99" t="inlineStr">
+        <is>
+          <t>https://washingtoncitypaper.com/article/766172/needle-deportation-trump-protests-no-kings/</t>
+        </is>
+      </c>
+      <c r="G99" t="n">
+        <v>-31</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B100" t="n">
+        <v>65</v>
+      </c>
+      <c r="C100" s="2" t="n">
+        <v>45821</v>
+      </c>
+      <c r="D100" t="n">
+        <v>2</v>
+      </c>
+      <c r="E100" t="n">
+        <v>-31</v>
+      </c>
+      <c r="F100" t="inlineStr">
+        <is>
+          <t>https://washingtoncitypaper.com/article/766120/the-needle-sen-padilla-cuffed-for-asking-questions-moco-students-walk-out-house-passes-another-anti-d-c-bill/</t>
+        </is>
+      </c>
+      <c r="G100" t="n">
+        <v>-33</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B101" t="n">
+        <v>64</v>
+      </c>
+      <c r="C101" s="2" t="n">
+        <v>45820</v>
+      </c>
+      <c r="D101" t="n">
+        <v>2</v>
+      </c>
+      <c r="E101" t="n">
+        <v>-33</v>
+      </c>
+      <c r="F101" t="inlineStr">
+        <is>
+          <t>https://washingtoncitypaper.com/article/766056/needle-trumps-drag-queens-kennedy-center/</t>
+        </is>
+      </c>
+      <c r="G101" t="n">
+        <v>-35</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B102" t="n">
+        <v>63</v>
+      </c>
+      <c r="C102" s="2" t="n">
+        <v>45819</v>
+      </c>
+      <c r="D102" t="n">
+        <v>2</v>
+      </c>
+      <c r="E102" t="n">
+        <v>-35</v>
+      </c>
+      <c r="F102" t="inlineStr">
+        <is>
+          <t>https://washingtoncitypaper.com/article/765993/the-needle-house-passes-two-anti-d-c-bills-anti-trump-protests-planned-this-weekend-and-nj-rep-indicted/</t>
+        </is>
+      </c>
+      <c r="G102" t="n">
+        <v>-37</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B103" t="n">
+        <v>62</v>
+      </c>
+      <c r="C103" s="2" t="n">
+        <v>45818</v>
+      </c>
+      <c r="D103" t="n">
+        <v>0</v>
+      </c>
+      <c r="E103" t="n">
+        <v>-37</v>
+      </c>
+      <c r="F103" t="inlineStr">
+        <is>
+          <t>https://washingtoncitypaper.com/article/765889/needle-road-closures-parade-bondi/</t>
+        </is>
+      </c>
+      <c r="G103" t="n">
+        <v>-37</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B104" t="n">
+        <v>61</v>
+      </c>
+      <c r="C104" s="2" t="n">
+        <v>45817</v>
+      </c>
+      <c r="D104" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E104" t="n">
+        <v>-37</v>
+      </c>
+      <c r="F104" t="inlineStr">
+        <is>
+          <t>https://washingtoncitypaper.com/article/765873/needle-kilmar-virginia-ice-trump-musk/</t>
+        </is>
+      </c>
+      <c r="G104" t="n">
+        <v>-36</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B105" t="n">
+        <v>60</v>
+      </c>
+      <c r="C105" s="2" t="n">
+        <v>45814</v>
+      </c>
+      <c r="D105" t="n">
+        <v>2</v>
+      </c>
+      <c r="E105" t="n">
+        <v>-36</v>
+      </c>
+      <c r="F105" t="inlineStr">
+        <is>
+          <t>https://washingtoncitypaper.com/article/765615/the-needle-the-end-of-the-trump-musk-bromance/</t>
+        </is>
+      </c>
+      <c r="G105" t="n">
+        <v>-39</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B106" t="n">
+        <v>59</v>
+      </c>
+      <c r="C106" s="2" t="n">
+        <v>45812</v>
+      </c>
+      <c r="D106" t="n">
+        <v>0</v>
+      </c>
+      <c r="E106" t="n">
+        <v>-39</v>
+      </c>
+      <c r="F106" t="inlineStr">
+        <is>
+          <t>https://washingtoncitypaper.com/article/765487/the-needle-butterworths-trans-health-care-prison-hegseth/</t>
+        </is>
+      </c>
+      <c r="G106" t="n">
+        <v>-39</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B107" t="n">
+        <v>58</v>
+      </c>
+      <c r="C107" s="2" t="n">
+        <v>45811</v>
+      </c>
+      <c r="D107" t="n">
+        <v>-3</v>
+      </c>
+      <c r="E107" t="n">
+        <v>-39</v>
+      </c>
+      <c r="F107" t="inlineStr">
+        <is>
+          <t>https://washingtoncitypaper.com/article/765245/the-needle-deportation-museum-latino/</t>
+        </is>
+      </c>
+      <c r="G107" t="n">
+        <v>-36</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B108" t="n">
+        <v>57</v>
+      </c>
+      <c r="C108" s="2" t="n">
+        <v>45810</v>
+      </c>
+      <c r="D108" t="n">
+        <v>-6</v>
+      </c>
+      <c r="E108" t="n">
+        <v>-36</v>
+      </c>
+      <c r="F108" t="inlineStr">
+        <is>
+          <t>https://washingtoncitypaper.com/article/765132/needle-rubio-afterschool-anacostia-community-museum/</t>
+        </is>
+      </c>
+      <c r="G108" t="n">
+        <v>-30</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B109" t="n">
+        <v>56</v>
+      </c>
+      <c r="C109" s="2" t="n">
+        <v>45807</v>
+      </c>
+      <c r="D109" t="n">
+        <v>-2</v>
+      </c>
+      <c r="E109" t="n">
+        <v>-30</v>
+      </c>
+      <c r="F109" t="inlineStr">
+        <is>
+          <t>https://washingtoncitypaper.com/article/765048/needle-supreme-court-immigration-trump-train/</t>
+        </is>
+      </c>
+      <c r="G109" t="n">
+        <v>-28</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B110" t="n">
+        <v>55</v>
+      </c>
+      <c r="C110" s="2" t="n">
+        <v>45806</v>
+      </c>
+      <c r="D110" t="n">
+        <v>4</v>
+      </c>
+      <c r="E110" t="n">
+        <v>-28</v>
+      </c>
+      <c r="F110" t="inlineStr">
+        <is>
+          <t>https://washingtoncitypaper.com/article/764968/needle-tariff-trump-musk/</t>
+        </is>
+      </c>
+      <c r="G110" t="n">
+        <v>-32</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B111" t="n">
+        <v>54</v>
+      </c>
+      <c r="C111" s="2" t="n">
+        <v>45805</v>
+      </c>
+      <c r="D111" t="n">
+        <v>-2</v>
+      </c>
+      <c r="E111" t="n">
+        <v>-32</v>
+      </c>
+      <c r="F111" t="inlineStr">
+        <is>
+          <t>https://washingtoncitypaper.com/article/764845/the-needle-trump-rains-on-worldpride-pardons-rich-friends-and-loses-to-the-lawyers/</t>
+        </is>
+      </c>
+      <c r="G111" t="n">
+        <v>-30</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B112" t="n">
+        <v>53</v>
+      </c>
+      <c r="C112" s="2" t="n">
+        <v>45804</v>
+      </c>
+      <c r="D112" t="n">
+        <v>-2</v>
+      </c>
+      <c r="E112" t="n">
+        <v>-30</v>
+      </c>
+      <c r="F112" t="inlineStr">
+        <is>
+          <t>https://washingtoncitypaper.com/article/764720/needle-jan-6-pardon-npr-sues-trump/</t>
+        </is>
+      </c>
+      <c r="G112" t="n">
+        <v>-28</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B113" t="n">
+        <v>52</v>
+      </c>
+      <c r="C113" s="2" t="n">
+        <v>45800</v>
+      </c>
+      <c r="D113" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E113" t="n">
+        <v>-28</v>
+      </c>
+      <c r="F113" t="inlineStr">
+        <is>
+          <t>https://washingtoncitypaper.com/article/764660/needle-spit-ed-martin-crypto/</t>
+        </is>
+      </c>
+      <c r="G113" t="n">
+        <v>-27</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B114" t="n">
+        <v>51</v>
+      </c>
+      <c r="C114" s="2" t="n">
+        <v>45799</v>
+      </c>
+      <c r="D114" t="n">
+        <v>4</v>
+      </c>
+      <c r="E114" t="n">
+        <v>-27</v>
+      </c>
+      <c r="F114" t="inlineStr">
+        <is>
+          <t>https://washingtoncitypaper.com/article/764538/needle-oval-military-parade-south-africa/</t>
+        </is>
+      </c>
+      <c r="G114" t="n">
+        <v>-31</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B115" t="n">
+        <v>50</v>
+      </c>
+      <c r="C115" s="2" t="n">
+        <v>45798</v>
+      </c>
+      <c r="D115" t="n">
+        <v>-6</v>
+      </c>
+      <c r="E115" t="n">
+        <v>-31</v>
+      </c>
+      <c r="F115" t="inlineStr">
+        <is>
+          <t>https://washingtoncitypaper.com/article/764398/needle-covid-habeas-corpus/</t>
+        </is>
+      </c>
+      <c r="G115" t="n">
+        <v>-25</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B116" t="n">
+        <v>49</v>
+      </c>
+      <c r="C116" s="2" t="n">
+        <v>45797</v>
+      </c>
+      <c r="D116" t="n">
+        <v>-7</v>
+      </c>
+      <c r="E116" t="n">
+        <v>-25</v>
+      </c>
+      <c r="F116" t="inlineStr">
+        <is>
+          <t>https://washingtoncitypaper.com/article/764351/needle-trump-doj-supreme-court/</t>
+        </is>
+      </c>
+      <c r="G116" t="n">
+        <v>-18</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B117" t="n">
+        <v>48</v>
+      </c>
+      <c r="C117" s="2" t="n">
+        <v>45796</v>
+      </c>
+      <c r="D117" t="n">
+        <v>-3</v>
+      </c>
+      <c r="E117" t="n">
+        <v>-18</v>
+      </c>
+      <c r="F117" t="inlineStr">
+        <is>
+          <t>https://washingtoncitypaper.com/article/764310/needle-arts-trump-doj-food-bank/</t>
+        </is>
+      </c>
+      <c r="G117" t="n">
+        <v>-15</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B118" t="n">
+        <v>47</v>
+      </c>
+      <c r="C118" s="2" t="n">
+        <v>45793</v>
+      </c>
+      <c r="D118" t="n">
+        <v>-2</v>
+      </c>
+      <c r="E118" t="n">
+        <v>-15</v>
+      </c>
+      <c r="F118" t="inlineStr">
+        <is>
+          <t>https://washingtoncitypaper.com/article/764207/needle-kennedy-center-military-parade/</t>
+        </is>
+      </c>
+      <c r="G118" t="n">
+        <v>-13</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B119" t="n">
+        <v>46</v>
+      </c>
+      <c r="C119" s="2" t="n">
+        <v>45792</v>
+      </c>
+      <c r="D119" t="n">
         <v>1</v>
       </c>
-      <c r="C96" s="2" t="n">
+      <c r="E119" t="n">
+        <v>-13</v>
+      </c>
+      <c r="F119" t="inlineStr">
+        <is>
+          <t>https://washingtoncitypaper.com/article/764120/needle-georgetown-student-protest-military-parade/</t>
+        </is>
+      </c>
+      <c r="G119" t="n">
+        <v>-14</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B120" t="n">
+        <v>45</v>
+      </c>
+      <c r="C120" s="2" t="n">
+        <v>45791</v>
+      </c>
+      <c r="D120" t="n">
+        <v>-2</v>
+      </c>
+      <c r="E120" t="n">
+        <v>-14</v>
+      </c>
+      <c r="F120" t="inlineStr">
+        <is>
+          <t>https://washingtoncitypaper.com/article/764040/needle-trump-rich-undocumented/</t>
+        </is>
+      </c>
+      <c r="G120" t="n">
+        <v>-12</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B121" t="n">
+        <v>44</v>
+      </c>
+      <c r="C121" s="2" t="n">
+        <v>45790</v>
+      </c>
+      <c r="D121" t="n">
+        <v>-4</v>
+      </c>
+      <c r="E121" t="n">
+        <v>-12</v>
+      </c>
+      <c r="F121" t="inlineStr">
+        <is>
+          <t>https://washingtoncitypaper.com/article/763944/needle-plane-trump-lawyer/</t>
+        </is>
+      </c>
+      <c r="G121" t="n">
+        <v>-8</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B122" t="n">
+        <v>43</v>
+      </c>
+      <c r="C122" s="2" t="n">
+        <v>45789</v>
+      </c>
+      <c r="D122" t="n">
+        <v>-5</v>
+      </c>
+      <c r="E122" t="n">
+        <v>-8</v>
+      </c>
+      <c r="F122" t="inlineStr">
+        <is>
+          <t>https://washingtoncitypaper.com/article/763841/the-needle-a-flying-palace-trump-fam-profits-off-crypto-and-ed-martin-fails-up/</t>
+        </is>
+      </c>
+      <c r="G122" t="n">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B123" t="n">
+        <v>42</v>
+      </c>
+      <c r="C123" s="2" t="n">
+        <v>45786</v>
+      </c>
+      <c r="D123" t="n">
+        <v>-3</v>
+      </c>
+      <c r="E123" t="n">
+        <v>-3</v>
+      </c>
+      <c r="F123" t="inlineStr">
+        <is>
+          <t>https://washingtoncitypaper.com/article/763748/needle-fired-feds-pentagon-trans-ban-carla-hayden/</t>
+        </is>
+      </c>
+      <c r="G123" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B124" t="n">
+        <v>41</v>
+      </c>
+      <c r="C124" s="2" t="n">
+        <v>45785</v>
+      </c>
+      <c r="D124" t="n">
+        <v>12</v>
+      </c>
+      <c r="E124" t="n">
+        <v>0</v>
+      </c>
+      <c r="F124" t="inlineStr">
+        <is>
+          <t>https://washingtoncitypaper.com/article/763697/needle-ed-martin-les-mis-cast/</t>
+        </is>
+      </c>
+      <c r="G124" t="n">
+        <v>-12</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B125" t="n">
+        <v>40</v>
+      </c>
+      <c r="C125" s="2" t="n">
+        <v>45784</v>
+      </c>
+      <c r="D125" t="n">
+        <v>-3</v>
+      </c>
+      <c r="E125" t="n">
+        <v>-12</v>
+      </c>
+      <c r="F125" t="inlineStr">
+        <is>
+          <t>https://washingtoncitypaper.com/article/763544/needle-supreme-trans-immigration-restaurants/</t>
+        </is>
+      </c>
+      <c r="G125" t="n">
+        <v>-9</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B126" t="n">
+        <v>39</v>
+      </c>
+      <c r="C126" s="2" t="n">
+        <v>45783</v>
+      </c>
+      <c r="D126" t="n">
+        <v>4</v>
+      </c>
+      <c r="E126" t="n">
+        <v>-9</v>
+      </c>
+      <c r="F126" t="inlineStr">
+        <is>
+          <t>https://washingtoncitypaper.com/article/763500/needle-deportation-dc-budget-ed-martin/</t>
+        </is>
+      </c>
+      <c r="G126" t="n">
+        <v>-13</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B127" t="n">
+        <v>38</v>
+      </c>
+      <c r="C127" s="2" t="n">
+        <v>45782</v>
+      </c>
+      <c r="D127" t="n">
+        <v>2</v>
+      </c>
+      <c r="E127" t="n">
+        <v>-13</v>
+      </c>
+      <c r="F127" t="inlineStr">
+        <is>
+          <t>https://washingtoncitypaper.com/article/763437/needle-trump-business-deal-ethics-constitution/</t>
+        </is>
+      </c>
+      <c r="G127" t="n">
+        <v>-15</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B128" t="n">
+        <v>37</v>
+      </c>
+      <c r="C128" s="2" t="n">
+        <v>45779</v>
+      </c>
+      <c r="D128" t="n">
+        <v>12</v>
+      </c>
+      <c r="E128" t="n">
+        <v>-15</v>
+      </c>
+      <c r="F128" t="inlineStr">
+        <is>
+          <t>https://washingtoncitypaper.com/article/763378/needle-ed-martin-deportations-doge/</t>
+        </is>
+      </c>
+      <c r="G128" t="n">
+        <v>-27</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B129" t="n">
+        <v>36</v>
+      </c>
+      <c r="C129" s="2" t="n">
+        <v>45778</v>
+      </c>
+      <c r="D129" t="n">
+        <v>2</v>
+      </c>
+      <c r="E129" t="n">
+        <v>-27</v>
+      </c>
+      <c r="F129" t="inlineStr">
+        <is>
+          <t>https://washingtoncitypaper.com/article/763329/needle-journalists-may-day-protests/</t>
+        </is>
+      </c>
+      <c r="G129" t="n">
+        <v>-29</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B130" t="n">
+        <v>35</v>
+      </c>
+      <c r="C130" s="2" t="n">
+        <v>45777</v>
+      </c>
+      <c r="D130" t="n">
+        <v>-5</v>
+      </c>
+      <c r="E130" t="n">
+        <v>-29</v>
+      </c>
+      <c r="F130" t="inlineStr">
+        <is>
+          <t>https://washingtoncitypaper.com/article/763223/needle-trump-kilmar-republicans-medicaid/</t>
+        </is>
+      </c>
+      <c r="G130" t="n">
+        <v>-24</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B131" t="n">
+        <v>34</v>
+      </c>
+      <c r="C131" s="2" t="n">
+        <v>45776</v>
+      </c>
+      <c r="D131" t="n">
+        <v>-5</v>
+      </c>
+      <c r="E131" t="n">
+        <v>-24</v>
+      </c>
+      <c r="F131" t="inlineStr">
+        <is>
+          <t>https://washingtoncitypaper.com/article/763129/needle-ed-martin-nazi/</t>
+        </is>
+      </c>
+      <c r="G131" t="n">
+        <v>-19</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B132" t="n">
+        <v>33</v>
+      </c>
+      <c r="C132" s="2" t="n">
+        <v>45775</v>
+      </c>
+      <c r="D132" t="n">
+        <v>2</v>
+      </c>
+      <c r="E132" t="n">
+        <v>-19</v>
+      </c>
+      <c r="F132" t="inlineStr">
+        <is>
+          <t>https://washingtoncitypaper.com/article/763081/the-needle-99-days-of-trump/</t>
+        </is>
+      </c>
+      <c r="G132" t="n">
+        <v>-15</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B133" t="n">
+        <v>32</v>
+      </c>
+      <c r="C133" s="2" t="n">
+        <v>45771</v>
+      </c>
+      <c r="D133" t="n">
+        <v>-3</v>
+      </c>
+      <c r="E133" t="n">
+        <v>-15</v>
+      </c>
+      <c r="F133" t="inlineStr">
+        <is>
+          <t>https://washingtoncitypaper.com/article/762919/needle-ed-martin-abrego-garcia-smithsonian/</t>
+        </is>
+      </c>
+      <c r="G133" t="n">
+        <v>-12</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B134" t="n">
+        <v>31</v>
+      </c>
+      <c r="C134" s="2" t="n">
+        <v>45770</v>
+      </c>
+      <c r="D134" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E134" t="n">
+        <v>-12</v>
+      </c>
+      <c r="F134" t="inlineStr">
+        <is>
+          <t>https://washingtoncitypaper.com/article/762817/needle-ed-martin-lgbtqia-hhs/</t>
+        </is>
+      </c>
+      <c r="G134" t="n">
+        <v>-11</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B135" t="n">
+        <v>30</v>
+      </c>
+      <c r="C135" s="2" t="n">
+        <v>45769</v>
+      </c>
+      <c r="D135" t="n">
+        <v>-11</v>
+      </c>
+      <c r="E135" t="n">
+        <v>-11</v>
+      </c>
+      <c r="F135" t="inlineStr">
+        <is>
+          <t>https://washingtoncitypaper.com/article/762704/needle-harvard-cancer-scientist/</t>
+        </is>
+      </c>
+      <c r="G135" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B136" t="n">
+        <v>29</v>
+      </c>
+      <c r="C136" s="2" t="n">
+        <v>45768</v>
+      </c>
+      <c r="D136" t="n">
+        <v>8</v>
+      </c>
+      <c r="E136" t="n">
+        <v>0</v>
+      </c>
+      <c r="F136" t="inlineStr">
+        <is>
+          <t>https://washingtoncitypaper.com/article/762610/needle-hegseth-supremecourt-immigration-deportation/</t>
+        </is>
+      </c>
+      <c r="G136" t="n">
+        <v>-8</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B137" t="n">
+        <v>28</v>
+      </c>
+      <c r="C137" s="2" t="n">
+        <v>45765</v>
+      </c>
+      <c r="D137" t="n">
+        <v>12</v>
+      </c>
+      <c r="E137" t="n">
+        <v>-8</v>
+      </c>
+      <c r="F137" t="inlineStr">
+        <is>
+          <t>https://washingtoncitypaper.com/article/762539/needle-kilmar-vanhollen/</t>
+        </is>
+      </c>
+      <c r="G137" t="n">
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B138" t="n">
+        <v>27</v>
+      </c>
+      <c r="C138" s="2" t="n">
+        <v>45764</v>
+      </c>
+      <c r="D138" t="n">
+        <v>-3</v>
+      </c>
+      <c r="E138" t="n">
+        <v>-20</v>
+      </c>
+      <c r="F138" t="inlineStr">
+        <is>
+          <t>https://washingtoncitypaper.com/article/762425/needle-van-hollen-harvard/</t>
+        </is>
+      </c>
+      <c r="G138" t="n">
+        <v>-8</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B139" t="n">
+        <v>26</v>
+      </c>
+      <c r="C139" s="2" t="n">
+        <v>45762</v>
+      </c>
+      <c r="D139" t="n">
+        <v>-2</v>
+      </c>
+      <c r="E139" t="n">
+        <v>-8</v>
+      </c>
+      <c r="F139" t="inlineStr">
+        <is>
+          <t>https://washingtoncitypaper.com/article/762198/needle-doge-data-nlrb-whistleblower/</t>
+        </is>
+      </c>
+      <c r="G139" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B140" t="n">
+        <v>25</v>
+      </c>
+      <c r="C140" s="2" t="n">
+        <v>45758</v>
+      </c>
+      <c r="D140" t="n">
+        <v>8</v>
+      </c>
+      <c r="E140" t="n">
+        <v>0</v>
+      </c>
+      <c r="F140" t="inlineStr">
+        <is>
+          <t>https://washingtoncitypaper.com/article/762084/needle-abregogarcia-ice-rubio-eggs/</t>
+        </is>
+      </c>
+      <c r="G140" t="n">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B141" t="n">
+        <v>24</v>
+      </c>
+      <c r="C141" s="2" t="n">
+        <v>45756</v>
+      </c>
+      <c r="D141" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E141" t="n">
+        <v>-5</v>
+      </c>
+      <c r="F141" t="inlineStr">
+        <is>
+          <t>https://washingtoncitypaper.com/article/762015/needle-press-pronouns-first-amendment/</t>
+        </is>
+      </c>
+      <c r="G141" t="n">
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B142" t="n">
+        <v>23</v>
+      </c>
+      <c r="C142" s="2" t="n">
+        <v>45755</v>
+      </c>
+      <c r="D142" t="n">
+        <v>-5</v>
+      </c>
+      <c r="E142" t="n">
+        <v>-4</v>
+      </c>
+      <c r="F142" t="inlineStr">
+        <is>
+          <t>https://washingtoncitypaper.com/article/761902/needle-negative-supreme-court/</t>
+        </is>
+      </c>
+      <c r="G142" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B143" t="n">
+        <v>22</v>
+      </c>
+      <c r="C143" s="2" t="n">
+        <v>45751</v>
+      </c>
+      <c r="D143" t="n">
+        <v>0</v>
+      </c>
+      <c r="E143" t="n">
+        <v>4</v>
+      </c>
+      <c r="F143" t="inlineStr">
+        <is>
+          <t>https://washingtoncitypaper.com/article/761750/needle-laura-loomer-trump/</t>
+        </is>
+      </c>
+      <c r="G143" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B144" t="n">
+        <v>21</v>
+      </c>
+      <c r="C144" s="2" t="n">
+        <v>45750</v>
+      </c>
+      <c r="D144" t="n">
+        <v>-5</v>
+      </c>
+      <c r="E144" t="n">
+        <v>4</v>
+      </c>
+      <c r="F144" t="inlineStr">
+        <is>
+          <t>https://washingtoncitypaper.com/article/761656/needle-trade-war-budget/</t>
+        </is>
+      </c>
+      <c r="G144" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B145" t="n">
+        <v>20</v>
+      </c>
+      <c r="C145" s="2" t="n">
+        <v>45749</v>
+      </c>
+      <c r="D145" t="n">
+        <v>4</v>
+      </c>
+      <c r="E145" t="n">
+        <v>9</v>
+      </c>
+      <c r="F145" t="inlineStr">
+        <is>
+          <t>https://washingtoncitypaper.com/article/761599/needle-booker-schiff-martin/</t>
+        </is>
+      </c>
+      <c r="G145" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B146" t="n">
+        <v>19</v>
+      </c>
+      <c r="C146" s="2" t="n">
+        <v>45748</v>
+      </c>
+      <c r="D146" t="n">
+        <v>-5</v>
+      </c>
+      <c r="E146" t="n">
+        <v>5</v>
+      </c>
+      <c r="F146" t="inlineStr">
+        <is>
+          <t>https://washingtoncitypaper.com/article/761505/needle-immigration-deportation-error/</t>
+        </is>
+      </c>
+      <c r="G146" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B147" t="n">
+        <v>18</v>
+      </c>
+      <c r="C147" s="2" t="n">
+        <v>45747</v>
+      </c>
+      <c r="D147" t="n">
+        <v>0</v>
+      </c>
+      <c r="E147" t="n">
+        <v>10</v>
+      </c>
+      <c r="F147" t="inlineStr">
+        <is>
+          <t>https://washingtoncitypaper.com/article/761408/needle-third-term/</t>
+        </is>
+      </c>
+      <c r="G147" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B148" t="n">
+        <v>17</v>
+      </c>
+      <c r="C148" s="2" t="n">
+        <v>45744</v>
+      </c>
+      <c r="D148" t="n">
+        <v>-12</v>
+      </c>
+      <c r="E148" t="n">
+        <v>10</v>
+      </c>
+      <c r="F148" t="inlineStr">
+        <is>
+          <t>https://washingtoncitypaper.com/article/761339/needle-trump-executive-order-public-safety/</t>
+        </is>
+      </c>
+      <c r="G148" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B149" t="n">
+        <v>16</v>
+      </c>
+      <c r="C149" s="2" t="n">
+        <v>45743</v>
+      </c>
+      <c r="D149" t="n">
+        <v>1</v>
+      </c>
+      <c r="E149" t="n">
+        <v>22</v>
+      </c>
+      <c r="F149" t="inlineStr">
+        <is>
+          <t>https://washingtoncitypaper.com/article/761265/needle-judge-boasberg-hdcooke-signal/</t>
+        </is>
+      </c>
+      <c r="G149" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B150" t="n">
+        <v>15</v>
+      </c>
+      <c r="C150" s="2" t="n">
+        <v>45742</v>
+      </c>
+      <c r="D150" t="n">
+        <v>-5</v>
+      </c>
+      <c r="E150" t="n">
+        <v>21</v>
+      </c>
+      <c r="F150" t="inlineStr">
+        <is>
+          <t>https://washingtoncitypaper.com/article/761141/the-needle-district-of-america-edition/</t>
+        </is>
+      </c>
+      <c r="G150" t="n">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B151" t="n">
+        <v>14</v>
+      </c>
+      <c r="C151" s="2" t="n">
+        <v>45741</v>
+      </c>
+      <c r="D151" t="n">
+        <v>0</v>
+      </c>
+      <c r="E151" t="n">
+        <v>26</v>
+      </c>
+      <c r="F151" t="inlineStr">
+        <is>
+          <t>https://washingtoncitypaper.com/article/761005/the-needle-group-chat-edition/</t>
+        </is>
+      </c>
+      <c r="G151" t="n">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B152" t="n">
+        <v>13</v>
+      </c>
+      <c r="C152" s="2" t="n">
+        <v>45740</v>
+      </c>
+      <c r="D152" t="n">
+        <v>-4</v>
+      </c>
+      <c r="E152" t="n">
+        <v>26</v>
+      </c>
+      <c r="F152" t="inlineStr">
+        <is>
+          <t>https://washingtoncitypaper.com/article/760917/needle-musk-ed-martin/</t>
+        </is>
+      </c>
+      <c r="G152" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B153" t="n">
+        <v>12</v>
+      </c>
+      <c r="C153" s="2" t="n">
+        <v>45737</v>
+      </c>
+      <c r="D153" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E153" t="n">
+        <v>30</v>
+      </c>
+      <c r="F153" t="inlineStr">
+        <is>
+          <t>https://washingtoncitypaper.com/article/760826/needle-trump-musk-deportation-immigrant-georgetown/</t>
+        </is>
+      </c>
+      <c r="G153" t="n">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B154" t="n">
+        <v>11</v>
+      </c>
+      <c r="C154" s="2" t="n">
+        <v>45736</v>
+      </c>
+      <c r="D154" t="n">
+        <v>-3</v>
+      </c>
+      <c r="E154" t="n">
+        <v>31</v>
+      </c>
+      <c r="F154" t="inlineStr">
+        <is>
+          <t>https://washingtoncitypaper.com/article/760736/needle-georgetown-immigration-tarrio/</t>
+        </is>
+      </c>
+      <c r="G154" t="n">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B155" t="n">
+        <v>10</v>
+      </c>
+      <c r="C155" s="2" t="n">
+        <v>45735</v>
+      </c>
+      <c r="D155" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E155" t="n">
+        <v>34</v>
+      </c>
+      <c r="F155" t="inlineStr">
+        <is>
+          <t>https://washingtoncitypaper.com/article/760643/the-needle-judgment-day-edition/</t>
+        </is>
+      </c>
+      <c r="G155" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B156" t="n">
+        <v>9</v>
+      </c>
+      <c r="C156" s="2" t="n">
+        <v>45734</v>
+      </c>
+      <c r="D156" t="n">
+        <v>1</v>
+      </c>
+      <c r="E156" t="n">
+        <v>35</v>
+      </c>
+      <c r="F156" t="inlineStr">
+        <is>
+          <t>https://washingtoncitypaper.com/article/760572/needle-semisonic-kennedy-center-trump/</t>
+        </is>
+      </c>
+      <c r="G156" t="n">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B157" t="n">
+        <v>8</v>
+      </c>
+      <c r="C157" s="2" t="n">
+        <v>45733</v>
+      </c>
+      <c r="D157" t="n">
+        <v>-5</v>
+      </c>
+      <c r="E157" t="n">
+        <v>34</v>
+      </c>
+      <c r="F157" t="inlineStr">
+        <is>
+          <t>https://washingtoncitypaper.com/article/760471/the-needle-deportation-budget/</t>
+        </is>
+      </c>
+      <c r="G157" t="n">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B158" t="n">
+        <v>7</v>
+      </c>
+      <c r="C158" s="2" t="n">
+        <v>45730</v>
+      </c>
+      <c r="D158" t="n">
+        <v>0</v>
+      </c>
+      <c r="E158" t="n">
+        <v>39</v>
+      </c>
+      <c r="F158" t="inlineStr">
+        <is>
+          <t>https://washingtoncitypaper.com/article/760390/needle-ed-martin-jd-vance-budget/</t>
+        </is>
+      </c>
+      <c r="G158" t="n">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B159" t="n">
+        <v>6</v>
+      </c>
+      <c r="C159" s="2" t="n">
+        <v>45729</v>
+      </c>
+      <c r="D159" t="n">
+        <v>2</v>
+      </c>
+      <c r="E159" t="n">
+        <v>39</v>
+      </c>
+      <c r="F159" t="inlineStr">
+        <is>
+          <t>https://washingtoncitypaper.com/article/760275/the-needle-musk-doge-budget/</t>
+        </is>
+      </c>
+      <c r="G159" t="n">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B160" t="n">
+        <v>5</v>
+      </c>
+      <c r="C160" s="2" t="n">
+        <v>45728</v>
+      </c>
+      <c r="D160" t="n">
+        <v>-9</v>
+      </c>
+      <c r="E160" t="n">
+        <v>37</v>
+      </c>
+      <c r="F160" t="inlineStr">
+        <is>
+          <t>https://washingtoncitypaper.com/article/760149/the-needle-retribution-watch-edition/</t>
+        </is>
+      </c>
+      <c r="G160" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B161" t="n">
+        <v>4</v>
+      </c>
+      <c r="C161" s="2" t="n">
+        <v>45727</v>
+      </c>
+      <c r="D161" t="n">
+        <v>2</v>
+      </c>
+      <c r="E161" t="n">
+        <v>46</v>
+      </c>
+      <c r="F161" t="inlineStr">
+        <is>
+          <t>https://washingtoncitypaper.com/article/760018/needle-budget-jobs/</t>
+        </is>
+      </c>
+      <c r="G161" t="n">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B162" t="n">
+        <v>3</v>
+      </c>
+      <c r="C162" s="2" t="n">
+        <v>45726</v>
+      </c>
+      <c r="D162" t="n">
+        <v>-13</v>
+      </c>
+      <c r="E162" t="n">
+        <v>44</v>
+      </c>
+      <c r="F162" t="inlineStr">
+        <is>
+          <t>https://washingtoncitypaper.com/article/759853/the-needle-budget-blow-up-edition/</t>
+        </is>
+      </c>
+      <c r="G162" t="n">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B163" t="n">
+        <v>2</v>
+      </c>
+      <c r="C163" s="2" t="n">
+        <v>45723</v>
+      </c>
+      <c r="D163" t="n">
+        <v>-11</v>
+      </c>
+      <c r="E163" t="n">
+        <v>57</v>
+      </c>
+      <c r="F163" t="inlineStr">
+        <is>
+          <t>https://washingtoncitypaper.com/article/759667/the-needle-capitulation-watch-edition/</t>
+        </is>
+      </c>
+      <c r="G163" t="n">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B164" t="n">
+        <v>1</v>
+      </c>
+      <c r="C164" s="2" t="n">
         <v>45722</v>
       </c>
-      <c r="D96" t="n">
+      <c r="D164" t="n">
         <v>-2</v>
       </c>
-      <c r="E96" t="n">
+      <c r="E164" t="n">
         <v>68</v>
       </c>
-      <c r="F96" t="inlineStr">
+      <c r="F164" t="inlineStr">
         <is>
           <t>https://washingtoncitypaper.com/article/759589/reintroducing-the-needle/</t>
         </is>
       </c>
-      <c r="G96" t="inlineStr"/>
+      <c r="G164" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
added day to the last update field
</commit_message>
<xml_diff>
--- a/input/scores.xlsx
+++ b/input/scores.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G164"/>
+  <dimension ref="A1:H164"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -468,6 +468,11 @@
           <t>needle_rating_previous</t>
         </is>
       </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>previous_test</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -493,6 +498,9 @@
       <c r="G2" t="n">
         <v>-325</v>
       </c>
+      <c r="H2" t="n">
+        <v>-325</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -518,6 +526,9 @@
       <c r="G3" t="n">
         <v>-320</v>
       </c>
+      <c r="H3" t="n">
+        <v>-295</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -543,6 +554,9 @@
       <c r="G4" t="n">
         <v>-313</v>
       </c>
+      <c r="H4" t="n">
+        <v>-313</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -568,6 +582,9 @@
       <c r="G5" t="n">
         <v>-298</v>
       </c>
+      <c r="H5" t="n">
+        <v>-298</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -593,6 +610,9 @@
       <c r="G6" t="n">
         <v>-290</v>
       </c>
+      <c r="H6" t="n">
+        <v>-290</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -618,6 +638,9 @@
       <c r="G7" t="n">
         <v>-272</v>
       </c>
+      <c r="H7" t="n">
+        <v>-272</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -643,6 +666,9 @@
       <c r="G8" t="n">
         <v>-279</v>
       </c>
+      <c r="H8" t="n">
+        <v>-279</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
@@ -668,6 +694,9 @@
       <c r="G9" t="n">
         <v>-293</v>
       </c>
+      <c r="H9" t="n">
+        <v>-292</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
@@ -693,6 +722,9 @@
       <c r="G10" t="n">
         <v>-301</v>
       </c>
+      <c r="H10" t="n">
+        <v>-301</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
@@ -718,6 +750,9 @@
       <c r="G11" t="n">
         <v>-292</v>
       </c>
+      <c r="H11" t="n">
+        <v>-292</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
@@ -743,6 +778,9 @@
       <c r="G12" t="n">
         <v>-282</v>
       </c>
+      <c r="H12" t="n">
+        <v>-289</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
@@ -768,6 +806,9 @@
       <c r="G13" t="n">
         <v>-273</v>
       </c>
+      <c r="H13" t="n">
+        <v>-281</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
@@ -793,6 +834,9 @@
       <c r="G14" t="n">
         <v>-277</v>
       </c>
+      <c r="H14" t="n">
+        <v>-266</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
@@ -818,6 +862,9 @@
       <c r="G15" t="n">
         <v>-269</v>
       </c>
+      <c r="H15" t="n">
+        <v>-269</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
@@ -843,6 +890,9 @@
       <c r="G16" t="n">
         <v>-260</v>
       </c>
+      <c r="H16" t="n">
+        <v>-260</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
@@ -868,6 +918,9 @@
       <c r="G17" t="n">
         <v>-248</v>
       </c>
+      <c r="H17" t="n">
+        <v>-248</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
@@ -893,6 +946,9 @@
       <c r="G18" t="n">
         <v>-244</v>
       </c>
+      <c r="H18" t="n">
+        <v>-244</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
@@ -918,6 +974,9 @@
       <c r="G19" t="n">
         <v>-239</v>
       </c>
+      <c r="H19" t="n">
+        <v>-239</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
@@ -943,6 +1002,9 @@
       <c r="G20" t="n">
         <v>-240</v>
       </c>
+      <c r="H20" t="n">
+        <v>-240</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
@@ -968,6 +1030,9 @@
       <c r="G21" t="n">
         <v>-231</v>
       </c>
+      <c r="H21" t="n">
+        <v>-231</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
@@ -993,6 +1058,9 @@
       <c r="G22" t="n">
         <v>-228</v>
       </c>
+      <c r="H22" t="n">
+        <v>-227</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
@@ -1018,6 +1086,9 @@
       <c r="G23" t="n">
         <v>-227</v>
       </c>
+      <c r="H23" t="n">
+        <v>-227</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
@@ -1043,6 +1114,9 @@
       <c r="G24" t="n">
         <v>-228</v>
       </c>
+      <c r="H24" t="n">
+        <v>-228</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
@@ -1068,6 +1142,9 @@
       <c r="G25" t="n">
         <v>-228</v>
       </c>
+      <c r="H25" t="n">
+        <v>-228</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
@@ -1093,6 +1170,9 @@
       <c r="G26" t="n">
         <v>-235</v>
       </c>
+      <c r="H26" t="n">
+        <v>-229</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
@@ -1118,6 +1198,9 @@
       <c r="G27" t="n">
         <v>-229</v>
       </c>
+      <c r="H27" t="n">
+        <v>-229</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
@@ -1143,6 +1226,9 @@
       <c r="G28" t="n">
         <v>-234</v>
       </c>
+      <c r="H28" t="n">
+        <v>-234</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
@@ -1168,6 +1254,9 @@
       <c r="G29" t="n">
         <v>-233</v>
       </c>
+      <c r="H29" t="n">
+        <v>-233</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
@@ -1193,6 +1282,9 @@
       <c r="G30" t="n">
         <v>-235</v>
       </c>
+      <c r="H30" t="n">
+        <v>-235</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
@@ -1218,6 +1310,9 @@
       <c r="G31" t="n">
         <v>-274</v>
       </c>
+      <c r="H31" t="n">
+        <v>-226</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
@@ -1243,6 +1338,9 @@
       <c r="G32" t="n">
         <v>-267</v>
       </c>
+      <c r="H32" t="n">
+        <v>-267</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
@@ -1268,6 +1366,9 @@
       <c r="G33" t="n">
         <v>-262</v>
       </c>
+      <c r="H33" t="n">
+        <v>-262</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
@@ -1293,6 +1394,9 @@
       <c r="G34" t="n">
         <v>-234</v>
       </c>
+      <c r="H34" t="n">
+        <v>-263</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
@@ -1318,6 +1422,9 @@
       <c r="G35" t="n">
         <v>-225</v>
       </c>
+      <c r="H35" t="n">
+        <v>-227</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
@@ -1343,6 +1450,9 @@
       <c r="G36" t="n">
         <v>-223</v>
       </c>
+      <c r="H36" t="n">
+        <v>-223</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
@@ -1368,6 +1478,9 @@
       <c r="G37" t="n">
         <v>-217</v>
       </c>
+      <c r="H37" t="n">
+        <v>-217</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
@@ -1393,6 +1506,9 @@
       <c r="G38" t="n">
         <v>-211</v>
       </c>
+      <c r="H38" t="n">
+        <v>-211</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
@@ -1418,6 +1534,9 @@
       <c r="G39" t="n">
         <v>-209</v>
       </c>
+      <c r="H39" t="n">
+        <v>-209</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
@@ -1443,6 +1562,9 @@
       <c r="G40" t="n">
         <v>-207</v>
       </c>
+      <c r="H40" t="n">
+        <v>-207</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
@@ -1468,6 +1590,9 @@
       <c r="G41" t="n">
         <v>-200</v>
       </c>
+      <c r="H41" t="n">
+        <v>-200</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
@@ -1493,6 +1618,9 @@
       <c r="G42" t="n">
         <v>-189</v>
       </c>
+      <c r="H42" t="n">
+        <v>-189</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
@@ -1518,6 +1646,9 @@
       <c r="G43" t="n">
         <v>-186</v>
       </c>
+      <c r="H43" t="n">
+        <v>-186</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
@@ -1543,6 +1674,9 @@
       <c r="G44" t="n">
         <v>-180</v>
       </c>
+      <c r="H44" t="n">
+        <v>-180</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
@@ -1568,6 +1702,9 @@
       <c r="G45" t="n">
         <v>-176</v>
       </c>
+      <c r="H45" t="n">
+        <v>-176</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
@@ -1593,6 +1730,9 @@
       <c r="G46" t="n">
         <v>-170</v>
       </c>
+      <c r="H46" t="n">
+        <v>-176</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
@@ -1618,6 +1758,9 @@
       <c r="G47" t="n">
         <v>-166</v>
       </c>
+      <c r="H47" t="n">
+        <v>-166</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
@@ -1643,6 +1786,9 @@
       <c r="G48" t="n">
         <v>-154</v>
       </c>
+      <c r="H48" t="n">
+        <v>-154</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
@@ -1668,6 +1814,9 @@
       <c r="G49" t="n">
         <v>-112</v>
       </c>
+      <c r="H49" t="n">
+        <v>-145</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
@@ -1693,6 +1842,9 @@
       <c r="G50" t="n">
         <v>-105</v>
       </c>
+      <c r="H50" t="n">
+        <v>-105</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
@@ -1718,6 +1870,9 @@
       <c r="G51" t="n">
         <v>-83</v>
       </c>
+      <c r="H51" t="n">
+        <v>-96</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="n">
@@ -1743,6 +1898,9 @@
       <c r="G52" t="n">
         <v>-70</v>
       </c>
+      <c r="H52" t="n">
+        <v>-76</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="n">
@@ -1768,6 +1926,9 @@
       <c r="G53" t="n">
         <v>-62</v>
       </c>
+      <c r="H53" t="n">
+        <v>-62</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="n">
@@ -1793,6 +1954,9 @@
       <c r="G54" t="n">
         <v>-61</v>
       </c>
+      <c r="H54" t="n">
+        <v>-61</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="n">
@@ -1818,6 +1982,9 @@
       <c r="G55" t="n">
         <v>-139</v>
       </c>
+      <c r="H55" t="n">
+        <v>-139</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="n">
@@ -1843,6 +2010,9 @@
       <c r="G56" t="n">
         <v>-136</v>
       </c>
+      <c r="H56" t="n">
+        <v>-136</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="n">
@@ -1868,6 +2038,9 @@
       <c r="G57" t="n">
         <v>-135</v>
       </c>
+      <c r="H57" t="n">
+        <v>-135</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="n">
@@ -1893,6 +2066,9 @@
       <c r="G58" t="n">
         <v>-134</v>
       </c>
+      <c r="H58" t="n">
+        <v>-137</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="n">
@@ -1918,6 +2094,9 @@
       <c r="G59" t="n">
         <v>-134</v>
       </c>
+      <c r="H59" t="n">
+        <v>-136</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="n">
@@ -1943,6 +2122,9 @@
       <c r="G60" t="n">
         <v>-129</v>
       </c>
+      <c r="H60" t="n">
+        <v>-134</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="n">
@@ -1968,6 +2150,9 @@
       <c r="G61" t="n">
         <v>-127</v>
       </c>
+      <c r="H61" t="n">
+        <v>-127</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="n">
@@ -1993,6 +2178,9 @@
       <c r="G62" t="n">
         <v>-121</v>
       </c>
+      <c r="H62" t="n">
+        <v>-121</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
@@ -2018,6 +2206,9 @@
       <c r="G63" t="n">
         <v>-118</v>
       </c>
+      <c r="H63" t="n">
+        <v>-112</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="n">
@@ -2043,6 +2234,9 @@
       <c r="G64" t="n">
         <v>-114</v>
       </c>
+      <c r="H64" t="n">
+        <v>-114</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="n">
@@ -2068,6 +2262,9 @@
       <c r="G65" t="n">
         <v>-112</v>
       </c>
+      <c r="H65" t="n">
+        <v>-112</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="n">
@@ -2093,6 +2290,9 @@
       <c r="G66" t="n">
         <v>-103</v>
       </c>
+      <c r="H66" t="n">
+        <v>-103</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="n">
@@ -2118,6 +2318,9 @@
       <c r="G67" t="n">
         <v>-98</v>
       </c>
+      <c r="H67" t="n">
+        <v>-98</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="n">
@@ -2143,6 +2346,9 @@
       <c r="G68" t="n">
         <v>-94</v>
       </c>
+      <c r="H68" t="n">
+        <v>-95</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="n">
@@ -2168,6 +2374,9 @@
       <c r="G69" t="n">
         <v>-90</v>
       </c>
+      <c r="H69" t="n">
+        <v>-90</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="n">
@@ -2193,6 +2402,9 @@
       <c r="G70" t="n">
         <v>-88</v>
       </c>
+      <c r="H70" t="n">
+        <v>-88</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="n">
@@ -2218,6 +2430,9 @@
       <c r="G71" t="n">
         <v>-76</v>
       </c>
+      <c r="H71" t="n">
+        <v>-82</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="n">
@@ -2243,6 +2458,9 @@
       <c r="G72" t="n">
         <v>-74</v>
       </c>
+      <c r="H72" t="n">
+        <v>-74</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="n">
@@ -2268,6 +2486,9 @@
       <c r="G73" t="n">
         <v>-68</v>
       </c>
+      <c r="H73" t="n">
+        <v>-68</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" s="1" t="n">
@@ -2293,6 +2514,9 @@
       <c r="G74" t="n">
         <v>-65</v>
       </c>
+      <c r="H74" t="n">
+        <v>-65</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75" s="1" t="n">
@@ -2318,6 +2542,9 @@
       <c r="G75" t="n">
         <v>-62</v>
       </c>
+      <c r="H75" t="n">
+        <v>-62</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" s="1" t="n">
@@ -2343,6 +2570,9 @@
       <c r="G76" t="n">
         <v>-62</v>
       </c>
+      <c r="H76" t="n">
+        <v>-62</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" s="1" t="n">
@@ -2368,6 +2598,9 @@
       <c r="G77" t="n">
         <v>-61</v>
       </c>
+      <c r="H77" t="n">
+        <v>-61</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" s="1" t="n">
@@ -2393,6 +2626,9 @@
       <c r="G78" t="n">
         <v>-66</v>
       </c>
+      <c r="H78" t="n">
+        <v>-63</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" s="1" t="n">
@@ -2418,6 +2654,9 @@
       <c r="G79" t="n">
         <v>-63</v>
       </c>
+      <c r="H79" t="n">
+        <v>-63</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" s="1" t="n">
@@ -2443,6 +2682,9 @@
       <c r="G80" t="n">
         <v>-61</v>
       </c>
+      <c r="H80" t="n">
+        <v>-61</v>
+      </c>
     </row>
     <row r="81">
       <c r="A81" s="1" t="n">
@@ -2468,6 +2710,9 @@
       <c r="G81" t="n">
         <v>-56</v>
       </c>
+      <c r="H81" t="n">
+        <v>-56</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82" s="1" t="n">
@@ -2493,6 +2738,9 @@
       <c r="G82" t="n">
         <v>-55</v>
       </c>
+      <c r="H82" t="n">
+        <v>-55</v>
+      </c>
     </row>
     <row r="83">
       <c r="A83" s="1" t="n">
@@ -2518,6 +2766,9 @@
       <c r="G83" t="n">
         <v>-56</v>
       </c>
+      <c r="H83" t="n">
+        <v>-56</v>
+      </c>
     </row>
     <row r="84">
       <c r="A84" s="1" t="n">
@@ -2543,6 +2794,9 @@
       <c r="G84" t="n">
         <v>-57</v>
       </c>
+      <c r="H84" t="n">
+        <v>-57</v>
+      </c>
     </row>
     <row r="85">
       <c r="A85" s="1" t="n">
@@ -2568,6 +2822,9 @@
       <c r="G85" t="n">
         <v>-63</v>
       </c>
+      <c r="H85" t="n">
+        <v>-57</v>
+      </c>
     </row>
     <row r="86">
       <c r="A86" s="1" t="n">
@@ -2593,6 +2850,9 @@
       <c r="G86" t="n">
         <v>-61</v>
       </c>
+      <c r="H86" t="n">
+        <v>-63</v>
+      </c>
     </row>
     <row r="87">
       <c r="A87" s="1" t="n">
@@ -2618,6 +2878,9 @@
       <c r="G87" t="n">
         <v>-54</v>
       </c>
+      <c r="H87" t="n">
+        <v>-57</v>
+      </c>
     </row>
     <row r="88">
       <c r="A88" s="1" t="n">
@@ -2643,6 +2906,9 @@
       <c r="G88" t="n">
         <v>-51</v>
       </c>
+      <c r="H88" t="n">
+        <v>-51</v>
+      </c>
     </row>
     <row r="89">
       <c r="A89" s="1" t="n">
@@ -2668,6 +2934,9 @@
       <c r="G89" t="n">
         <v>-49</v>
       </c>
+      <c r="H89" t="n">
+        <v>-49</v>
+      </c>
     </row>
     <row r="90">
       <c r="A90" s="1" t="n">
@@ -2693,6 +2962,9 @@
       <c r="G90" t="n">
         <v>-46</v>
       </c>
+      <c r="H90" t="n">
+        <v>-46</v>
+      </c>
     </row>
     <row r="91">
       <c r="A91" s="1" t="n">
@@ -2718,6 +2990,9 @@
       <c r="G91" t="n">
         <v>-39</v>
       </c>
+      <c r="H91" t="n">
+        <v>-39</v>
+      </c>
     </row>
     <row r="92">
       <c r="A92" s="1" t="n">
@@ -2743,6 +3018,9 @@
       <c r="G92" t="n">
         <v>-32</v>
       </c>
+      <c r="H92" t="n">
+        <v>-32</v>
+      </c>
     </row>
     <row r="93">
       <c r="A93" s="1" t="n">
@@ -2768,6 +3046,9 @@
       <c r="G93" t="n">
         <v>-31</v>
       </c>
+      <c r="H93" t="n">
+        <v>-31</v>
+      </c>
     </row>
     <row r="94">
       <c r="A94" s="1" t="n">
@@ -2793,6 +3074,9 @@
       <c r="G94" t="n">
         <v>-34</v>
       </c>
+      <c r="H94" t="n">
+        <v>-34</v>
+      </c>
     </row>
     <row r="95">
       <c r="A95" s="1" t="n">
@@ -2818,6 +3102,9 @@
       <c r="G95" t="n">
         <v>-32</v>
       </c>
+      <c r="H95" t="n">
+        <v>-32</v>
+      </c>
     </row>
     <row r="96">
       <c r="A96" s="1" t="n">
@@ -2843,6 +3130,9 @@
       <c r="G96" t="n">
         <v>-35</v>
       </c>
+      <c r="H96" t="n">
+        <v>-29</v>
+      </c>
     </row>
     <row r="97">
       <c r="A97" s="1" t="n">
@@ -2868,6 +3158,9 @@
       <c r="G97" t="n">
         <v>-29</v>
       </c>
+      <c r="H97" t="n">
+        <v>-29</v>
+      </c>
     </row>
     <row r="98">
       <c r="A98" s="1" t="n">
@@ -2893,6 +3186,9 @@
       <c r="G98" t="n">
         <v>-26</v>
       </c>
+      <c r="H98" t="n">
+        <v>-26</v>
+      </c>
     </row>
     <row r="99">
       <c r="A99" s="1" t="n">
@@ -2918,6 +3214,9 @@
       <c r="G99" t="n">
         <v>-31</v>
       </c>
+      <c r="H99" t="n">
+        <v>-33</v>
+      </c>
     </row>
     <row r="100">
       <c r="A100" s="1" t="n">
@@ -2943,6 +3242,9 @@
       <c r="G100" t="n">
         <v>-33</v>
       </c>
+      <c r="H100" t="n">
+        <v>-33</v>
+      </c>
     </row>
     <row r="101">
       <c r="A101" s="1" t="n">
@@ -2968,6 +3270,9 @@
       <c r="G101" t="n">
         <v>-35</v>
       </c>
+      <c r="H101" t="n">
+        <v>-35</v>
+      </c>
     </row>
     <row r="102">
       <c r="A102" s="1" t="n">
@@ -2993,6 +3298,9 @@
       <c r="G102" t="n">
         <v>-37</v>
       </c>
+      <c r="H102" t="n">
+        <v>-37</v>
+      </c>
     </row>
     <row r="103">
       <c r="A103" s="1" t="n">
@@ -3018,6 +3326,9 @@
       <c r="G103" t="n">
         <v>-37</v>
       </c>
+      <c r="H103" t="n">
+        <v>-37</v>
+      </c>
     </row>
     <row r="104">
       <c r="A104" s="1" t="n">
@@ -3043,6 +3354,9 @@
       <c r="G104" t="n">
         <v>-36</v>
       </c>
+      <c r="H104" t="n">
+        <v>-36</v>
+      </c>
     </row>
     <row r="105">
       <c r="A105" s="1" t="n">
@@ -3068,6 +3382,9 @@
       <c r="G105" t="n">
         <v>-39</v>
       </c>
+      <c r="H105" t="n">
+        <v>-38</v>
+      </c>
     </row>
     <row r="106">
       <c r="A106" s="1" t="n">
@@ -3093,6 +3410,9 @@
       <c r="G106" t="n">
         <v>-39</v>
       </c>
+      <c r="H106" t="n">
+        <v>-39</v>
+      </c>
     </row>
     <row r="107">
       <c r="A107" s="1" t="n">
@@ -3118,6 +3438,9 @@
       <c r="G107" t="n">
         <v>-36</v>
       </c>
+      <c r="H107" t="n">
+        <v>-36</v>
+      </c>
     </row>
     <row r="108">
       <c r="A108" s="1" t="n">
@@ -3143,6 +3466,9 @@
       <c r="G108" t="n">
         <v>-30</v>
       </c>
+      <c r="H108" t="n">
+        <v>-30</v>
+      </c>
     </row>
     <row r="109">
       <c r="A109" s="1" t="n">
@@ -3168,6 +3494,9 @@
       <c r="G109" t="n">
         <v>-28</v>
       </c>
+      <c r="H109" t="n">
+        <v>-28</v>
+      </c>
     </row>
     <row r="110">
       <c r="A110" s="1" t="n">
@@ -3193,6 +3522,9 @@
       <c r="G110" t="n">
         <v>-32</v>
       </c>
+      <c r="H110" t="n">
+        <v>-32</v>
+      </c>
     </row>
     <row r="111">
       <c r="A111" s="1" t="n">
@@ -3218,6 +3550,9 @@
       <c r="G111" t="n">
         <v>-30</v>
       </c>
+      <c r="H111" t="n">
+        <v>-30</v>
+      </c>
     </row>
     <row r="112">
       <c r="A112" s="1" t="n">
@@ -3243,6 +3578,9 @@
       <c r="G112" t="n">
         <v>-28</v>
       </c>
+      <c r="H112" t="n">
+        <v>-28</v>
+      </c>
     </row>
     <row r="113">
       <c r="A113" s="1" t="n">
@@ -3268,6 +3606,9 @@
       <c r="G113" t="n">
         <v>-27</v>
       </c>
+      <c r="H113" t="n">
+        <v>-27</v>
+      </c>
     </row>
     <row r="114">
       <c r="A114" s="1" t="n">
@@ -3293,6 +3634,9 @@
       <c r="G114" t="n">
         <v>-31</v>
       </c>
+      <c r="H114" t="n">
+        <v>-31</v>
+      </c>
     </row>
     <row r="115">
       <c r="A115" s="1" t="n">
@@ -3318,6 +3662,9 @@
       <c r="G115" t="n">
         <v>-25</v>
       </c>
+      <c r="H115" t="n">
+        <v>-25</v>
+      </c>
     </row>
     <row r="116">
       <c r="A116" s="1" t="n">
@@ -3343,6 +3690,9 @@
       <c r="G116" t="n">
         <v>-18</v>
       </c>
+      <c r="H116" t="n">
+        <v>-18</v>
+      </c>
     </row>
     <row r="117">
       <c r="A117" s="1" t="n">
@@ -3368,6 +3718,9 @@
       <c r="G117" t="n">
         <v>-15</v>
       </c>
+      <c r="H117" t="n">
+        <v>-15</v>
+      </c>
     </row>
     <row r="118">
       <c r="A118" s="1" t="n">
@@ -3393,6 +3746,9 @@
       <c r="G118" t="n">
         <v>-13</v>
       </c>
+      <c r="H118" t="n">
+        <v>-13</v>
+      </c>
     </row>
     <row r="119">
       <c r="A119" s="1" t="n">
@@ -3418,6 +3774,9 @@
       <c r="G119" t="n">
         <v>-14</v>
       </c>
+      <c r="H119" t="n">
+        <v>-14</v>
+      </c>
     </row>
     <row r="120">
       <c r="A120" s="1" t="n">
@@ -3443,6 +3802,9 @@
       <c r="G120" t="n">
         <v>-12</v>
       </c>
+      <c r="H120" t="n">
+        <v>-12</v>
+      </c>
     </row>
     <row r="121">
       <c r="A121" s="1" t="n">
@@ -3468,6 +3830,9 @@
       <c r="G121" t="n">
         <v>-8</v>
       </c>
+      <c r="H121" t="n">
+        <v>-8</v>
+      </c>
     </row>
     <row r="122">
       <c r="A122" s="1" t="n">
@@ -3493,6 +3858,9 @@
       <c r="G122" t="n">
         <v>-3</v>
       </c>
+      <c r="H122" t="n">
+        <v>-3</v>
+      </c>
     </row>
     <row r="123">
       <c r="A123" s="1" t="n">
@@ -3518,6 +3886,9 @@
       <c r="G123" t="n">
         <v>0</v>
       </c>
+      <c r="H123" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="124">
       <c r="A124" s="1" t="n">
@@ -3543,6 +3914,9 @@
       <c r="G124" t="n">
         <v>-12</v>
       </c>
+      <c r="H124" t="n">
+        <v>-12</v>
+      </c>
     </row>
     <row r="125">
       <c r="A125" s="1" t="n">
@@ -3568,6 +3942,9 @@
       <c r="G125" t="n">
         <v>-9</v>
       </c>
+      <c r="H125" t="n">
+        <v>-9</v>
+      </c>
     </row>
     <row r="126">
       <c r="A126" s="1" t="n">
@@ -3593,6 +3970,9 @@
       <c r="G126" t="n">
         <v>-13</v>
       </c>
+      <c r="H126" t="n">
+        <v>-13</v>
+      </c>
     </row>
     <row r="127">
       <c r="A127" s="1" t="n">
@@ -3618,6 +3998,9 @@
       <c r="G127" t="n">
         <v>-15</v>
       </c>
+      <c r="H127" t="n">
+        <v>-15</v>
+      </c>
     </row>
     <row r="128">
       <c r="A128" s="1" t="n">
@@ -3643,6 +4026,9 @@
       <c r="G128" t="n">
         <v>-27</v>
       </c>
+      <c r="H128" t="n">
+        <v>-27</v>
+      </c>
     </row>
     <row r="129">
       <c r="A129" s="1" t="n">
@@ -3668,6 +4054,9 @@
       <c r="G129" t="n">
         <v>-29</v>
       </c>
+      <c r="H129" t="n">
+        <v>-29</v>
+      </c>
     </row>
     <row r="130">
       <c r="A130" s="1" t="n">
@@ -3693,6 +4082,9 @@
       <c r="G130" t="n">
         <v>-24</v>
       </c>
+      <c r="H130" t="n">
+        <v>-24</v>
+      </c>
     </row>
     <row r="131">
       <c r="A131" s="1" t="n">
@@ -3718,6 +4110,9 @@
       <c r="G131" t="n">
         <v>-19</v>
       </c>
+      <c r="H131" t="n">
+        <v>-19</v>
+      </c>
     </row>
     <row r="132">
       <c r="A132" s="1" t="n">
@@ -3743,6 +4138,9 @@
       <c r="G132" t="n">
         <v>-15</v>
       </c>
+      <c r="H132" t="n">
+        <v>-21</v>
+      </c>
     </row>
     <row r="133">
       <c r="A133" s="1" t="n">
@@ -3768,6 +4166,9 @@
       <c r="G133" t="n">
         <v>-12</v>
       </c>
+      <c r="H133" t="n">
+        <v>-12</v>
+      </c>
     </row>
     <row r="134">
       <c r="A134" s="1" t="n">
@@ -3793,6 +4194,9 @@
       <c r="G134" t="n">
         <v>-11</v>
       </c>
+      <c r="H134" t="n">
+        <v>-11</v>
+      </c>
     </row>
     <row r="135">
       <c r="A135" s="1" t="n">
@@ -3818,6 +4222,9 @@
       <c r="G135" t="n">
         <v>0</v>
       </c>
+      <c r="H135" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="136">
       <c r="A136" s="1" t="n">
@@ -3843,6 +4250,9 @@
       <c r="G136" t="n">
         <v>-8</v>
       </c>
+      <c r="H136" t="n">
+        <v>-8</v>
+      </c>
     </row>
     <row r="137">
       <c r="A137" s="1" t="n">
@@ -3868,6 +4278,9 @@
       <c r="G137" t="n">
         <v>-20</v>
       </c>
+      <c r="H137" t="n">
+        <v>-20</v>
+      </c>
     </row>
     <row r="138">
       <c r="A138" s="1" t="n">
@@ -3893,6 +4306,9 @@
       <c r="G138" t="n">
         <v>-8</v>
       </c>
+      <c r="H138" t="n">
+        <v>-17</v>
+      </c>
     </row>
     <row r="139">
       <c r="A139" s="1" t="n">
@@ -3918,6 +4334,9 @@
       <c r="G139" t="n">
         <v>0</v>
       </c>
+      <c r="H139" t="n">
+        <v>-6</v>
+      </c>
     </row>
     <row r="140">
       <c r="A140" s="1" t="n">
@@ -3943,6 +4362,9 @@
       <c r="G140" t="n">
         <v>-5</v>
       </c>
+      <c r="H140" t="n">
+        <v>-8</v>
+      </c>
     </row>
     <row r="141">
       <c r="A141" s="1" t="n">
@@ -3968,6 +4390,9 @@
       <c r="G141" t="n">
         <v>-4</v>
       </c>
+      <c r="H141" t="n">
+        <v>-4</v>
+      </c>
     </row>
     <row r="142">
       <c r="A142" s="1" t="n">
@@ -3993,6 +4418,9 @@
       <c r="G142" t="n">
         <v>4</v>
       </c>
+      <c r="H142" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="143">
       <c r="A143" s="1" t="n">
@@ -4018,6 +4446,9 @@
       <c r="G143" t="n">
         <v>4</v>
       </c>
+      <c r="H143" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="144">
       <c r="A144" s="1" t="n">
@@ -4043,6 +4474,9 @@
       <c r="G144" t="n">
         <v>9</v>
       </c>
+      <c r="H144" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="145">
       <c r="A145" s="1" t="n">
@@ -4068,6 +4502,9 @@
       <c r="G145" t="n">
         <v>5</v>
       </c>
+      <c r="H145" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="146">
       <c r="A146" s="1" t="n">
@@ -4093,6 +4530,9 @@
       <c r="G146" t="n">
         <v>10</v>
       </c>
+      <c r="H146" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="147">
       <c r="A147" s="1" t="n">
@@ -4118,6 +4558,9 @@
       <c r="G147" t="n">
         <v>10</v>
       </c>
+      <c r="H147" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="148">
       <c r="A148" s="1" t="n">
@@ -4143,6 +4586,9 @@
       <c r="G148" t="n">
         <v>22</v>
       </c>
+      <c r="H148" t="n">
+        <v>22</v>
+      </c>
     </row>
     <row r="149">
       <c r="A149" s="1" t="n">
@@ -4168,6 +4614,9 @@
       <c r="G149" t="n">
         <v>21</v>
       </c>
+      <c r="H149" t="n">
+        <v>21</v>
+      </c>
     </row>
     <row r="150">
       <c r="A150" s="1" t="n">
@@ -4193,6 +4642,9 @@
       <c r="G150" t="n">
         <v>26</v>
       </c>
+      <c r="H150" t="n">
+        <v>26</v>
+      </c>
     </row>
     <row r="151">
       <c r="A151" s="1" t="n">
@@ -4218,6 +4670,9 @@
       <c r="G151" t="n">
         <v>26</v>
       </c>
+      <c r="H151" t="n">
+        <v>26</v>
+      </c>
     </row>
     <row r="152">
       <c r="A152" s="1" t="n">
@@ -4243,6 +4698,9 @@
       <c r="G152" t="n">
         <v>30</v>
       </c>
+      <c r="H152" t="n">
+        <v>30</v>
+      </c>
     </row>
     <row r="153">
       <c r="A153" s="1" t="n">
@@ -4268,6 +4726,9 @@
       <c r="G153" t="n">
         <v>31</v>
       </c>
+      <c r="H153" t="n">
+        <v>31</v>
+      </c>
     </row>
     <row r="154">
       <c r="A154" s="1" t="n">
@@ -4293,6 +4754,9 @@
       <c r="G154" t="n">
         <v>34</v>
       </c>
+      <c r="H154" t="n">
+        <v>34</v>
+      </c>
     </row>
     <row r="155">
       <c r="A155" s="1" t="n">
@@ -4318,6 +4782,9 @@
       <c r="G155" t="n">
         <v>35</v>
       </c>
+      <c r="H155" t="n">
+        <v>35</v>
+      </c>
     </row>
     <row r="156">
       <c r="A156" s="1" t="n">
@@ -4343,6 +4810,9 @@
       <c r="G156" t="n">
         <v>34</v>
       </c>
+      <c r="H156" t="n">
+        <v>34</v>
+      </c>
     </row>
     <row r="157">
       <c r="A157" s="1" t="n">
@@ -4368,6 +4838,9 @@
       <c r="G157" t="n">
         <v>39</v>
       </c>
+      <c r="H157" t="n">
+        <v>39</v>
+      </c>
     </row>
     <row r="158">
       <c r="A158" s="1" t="n">
@@ -4393,6 +4866,9 @@
       <c r="G158" t="n">
         <v>39</v>
       </c>
+      <c r="H158" t="n">
+        <v>39</v>
+      </c>
     </row>
     <row r="159">
       <c r="A159" s="1" t="n">
@@ -4418,6 +4894,9 @@
       <c r="G159" t="n">
         <v>37</v>
       </c>
+      <c r="H159" t="n">
+        <v>37</v>
+      </c>
     </row>
     <row r="160">
       <c r="A160" s="1" t="n">
@@ -4443,6 +4922,9 @@
       <c r="G160" t="n">
         <v>46</v>
       </c>
+      <c r="H160" t="n">
+        <v>46</v>
+      </c>
     </row>
     <row r="161">
       <c r="A161" s="1" t="n">
@@ -4468,6 +4950,9 @@
       <c r="G161" t="n">
         <v>44</v>
       </c>
+      <c r="H161" t="n">
+        <v>44</v>
+      </c>
     </row>
     <row r="162">
       <c r="A162" s="1" t="n">
@@ -4493,6 +4978,9 @@
       <c r="G162" t="n">
         <v>57</v>
       </c>
+      <c r="H162" t="n">
+        <v>57</v>
+      </c>
     </row>
     <row r="163">
       <c r="A163" s="1" t="n">
@@ -4518,6 +5006,9 @@
       <c r="G163" t="n">
         <v>68</v>
       </c>
+      <c r="H163" t="n">
+        <v>68</v>
+      </c>
     </row>
     <row r="164">
       <c r="A164" s="1" t="n">
@@ -4541,6 +5032,9 @@
         </is>
       </c>
       <c r="G164" t="inlineStr"/>
+      <c r="H164" t="n">
+        <v>70</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>